<commit_message>
Added death of recent case from Hebei
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="18260" windowHeight="19000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -1174,8 +1174,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1195,7 +1197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1203,6 +1205,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1210,6 +1213,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1544,7 +1548,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="C143" sqref="C143"/>
+      <selection pane="bottomLeft" activeCell="M140" sqref="M140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7134,6 +7138,9 @@
       <c r="K137" s="1">
         <v>40003</v>
       </c>
+      <c r="L137" s="1">
+        <v>40039</v>
+      </c>
       <c r="M137" s="1">
         <v>40013</v>
       </c>

</xml_diff>

<commit_message>
New case in Hong Kong
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="384">
   <si>
     <t>gender</t>
   </si>
@@ -1156,6 +1156,21 @@
   </si>
   <si>
     <t>http://news.xinhuanet.com/english/china/2013-11/28/c_132925674.htm?utm_source=dlvr.it&amp;utm_medium=gplus</t>
+  </si>
+  <si>
+    <t>Shenzhen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guangdong </t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>The worker, 36, recently travelled to Shenzhen in the mainland and came into contact with live poultry. She is in critical condition, officials say.</t>
+  </si>
+  <si>
+    <t>http://www.bbc.co.uk/news/world-asia-china-25181387</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1229,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1268,7 +1287,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1292,6 +1311,8 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1315,6 +1336,8 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1644,12 +1667,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R143"/>
+  <dimension ref="A1:R144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="M145" sqref="M145"/>
+      <selection pane="bottomLeft" activeCell="N146" sqref="N146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6331,6 +6354,32 @@
         <v>378</v>
       </c>
     </row>
+    <row r="144" spans="1:18">
+      <c r="A144" t="s">
+        <v>22</v>
+      </c>
+      <c r="B144">
+        <v>36</v>
+      </c>
+      <c r="C144" t="s">
+        <v>380</v>
+      </c>
+      <c r="D144" t="s">
+        <v>379</v>
+      </c>
+      <c r="F144" t="s">
+        <v>381</v>
+      </c>
+      <c r="J144" s="1">
+        <v>40149</v>
+      </c>
+      <c r="K144" t="s">
+        <v>382</v>
+      </c>
+      <c r="N144" t="s">
+        <v>383</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
New case in HK
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="1820" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="386">
   <si>
     <t>gender</t>
   </si>
@@ -1171,6 +1171,17 @@
   </si>
   <si>
     <t>http://www.bbc.co.uk/news/world-asia-china-25181387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Centre for Health Protection (CHP) of the Department of Health (DH) is today (December 6) investigating another confirmed human case of avian influenza A(H7N9) in Hong Kong affecting a man aged 80.
+     The patient, with underlying medical condition, lives in Shenzhen. He was admitted to a hospital in Shenzhen for management of his chronic illness from November 13 to 29.
+     On December 3, he arrived in Hong Kong with his three family members via Shenzhen Bay Port Border Control Point (SBP BCP) and subsequently took a taxi there in the afternoon to the Accident and Emergency Department (AED) of Tuen Mun Hospital (TMH) where he was admitted for further management of his chronic illness on the same day.
+     The patient had no fever upon admission. However, he developed fever this morning and was put under isolation immediately. His nasopharyngeal swab was tested positive for the avian influenza A(H7N9) virus upon laboratory testing by the Public Health Laboratory Services Branch of the CHP today.
+     The patient will be transferred to Princess Margaret Hospital for isolation. His current condition is stable.
+</t>
+  </si>
+  <si>
+    <t>http://www.chp.gov.hk/en/content/116/32486.html</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1281,13 +1292,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1313,6 +1333,9 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1338,6 +1361,9 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1667,12 +1693,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R144"/>
+  <dimension ref="A1:R145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="N146" sqref="N146"/>
+      <selection pane="bottomLeft" activeCell="N145" sqref="N145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1680,6 +1706,7 @@
     <col min="7" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="23.1640625" style="1" customWidth="1"/>
     <col min="9" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -6378,6 +6405,38 @@
       </c>
       <c r="N144" t="s">
         <v>383</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" ht="15" customHeight="1">
+      <c r="A145" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145">
+        <v>80</v>
+      </c>
+      <c r="C145" t="s">
+        <v>380</v>
+      </c>
+      <c r="D145" t="s">
+        <v>379</v>
+      </c>
+      <c r="F145" t="s">
+        <v>381</v>
+      </c>
+      <c r="G145" s="1">
+        <v>40149</v>
+      </c>
+      <c r="H145" s="1">
+        <v>40149</v>
+      </c>
+      <c r="J145" s="1">
+        <v>40152</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="N145" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update and new case
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="390">
   <si>
     <t>gender</t>
   </si>
@@ -1182,7 +1182,13 @@
     <t>Authorities in south China's Guangdong province confirmed a new H7N9 bird flu case on Sunday. A 39-year-old man, surnamed He, has been hospitalized and is in serious condition, the provincial health authorities said in a statement. The statement said the resident in Dongguan City tested positive for the virus on Saturday in a local hospital, and the result was confirmed on Sunday by the provincial disease control center. No abnormity has been reported from the 53 people who had close contact with the patient, it said.</t>
   </si>
   <si>
-    <t>http://www.ecns.cn/2013/12-16/92728.shtml</t>
+    <t>http://beta.promedmail.org/direct.php?id=20131216.2118607</t>
+  </si>
+  <si>
+    <t>Yangjiang</t>
+  </si>
+  <si>
+    <t>http://www.shanghaidaily.com/national/Guangdong-confirms-2nd-H7N9-bird-flu-case/shdaily.shtml#jtss-twitter</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1247,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1316,7 +1330,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1349,6 +1363,10 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1381,6 +1399,10 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1710,12 +1732,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S147"/>
+  <dimension ref="A1:S148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="E147" sqref="E147"/>
+      <selection pane="bottomLeft" activeCell="O148" sqref="O148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6954,6 +6976,9 @@
       <c r="E147" t="s">
         <v>370</v>
       </c>
+      <c r="H147" s="1">
+        <v>40152</v>
+      </c>
       <c r="K147" s="1">
         <v>40160</v>
       </c>
@@ -6962,6 +6987,29 @@
       </c>
       <c r="O147" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148">
+        <v>65</v>
+      </c>
+      <c r="D148" t="s">
+        <v>353</v>
+      </c>
+      <c r="E148" t="s">
+        <v>388</v>
+      </c>
+      <c r="K148" s="1">
+        <v>40162</v>
+      </c>
+      <c r="O148" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#H7N9: Added 2 new cases and updated city coordinates
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="402">
   <si>
     <t>gender</t>
   </si>
@@ -894,9 +894,6 @@
     <t>#109 - Man, 91, onset on April 14, Tianchang, Chuzhou City, in hospital for treatment. Anhui province</t>
   </si>
   <si>
-    <t>Suzhou,</t>
-  </si>
-  <si>
     <t>citizen of Taiwan &amp; hospitalized there 2013-04-16, infected in Suzhou, was working in Jiangsu province and infected there</t>
   </si>
   <si>
@@ -927,18 +924,12 @@
     <t xml:space="preserve">#112 - Man, 56, onset date April 17, Zhongyuan district, Zhengzhou city, Henan province </t>
   </si>
   <si>
-    <t>Huzhou,</t>
-  </si>
-  <si>
     <t>Huzhou, Zhejiang province</t>
   </si>
   <si>
     <t>#113 - Woman, 60, farmer, onset April 17, Huzhou, Zhejiang province</t>
   </si>
   <si>
-    <t>Shaoxing,</t>
-  </si>
-  <si>
     <t>Shaoxing, Zhejiang province</t>
   </si>
   <si>
@@ -969,9 +960,6 @@
     <t>#117 - Man, 49, onset date April 17, Lishui Jiangsu province</t>
   </si>
   <si>
-    <t>Xuzhou Xinyi</t>
-  </si>
-  <si>
     <t>Xuzhou Xinyi City Jiangsu province</t>
   </si>
   <si>
@@ -1029,12 +1017,6 @@
     <t xml:space="preserve">#125 - Man, 38, onset on April 18. Currently the patient is hospitalized, seriously ill. Hangzhou Zhejiang province </t>
   </si>
   <si>
-    <t>Yang Fuqing</t>
-  </si>
-  <si>
-    <t>Fuzhou,</t>
-  </si>
-  <si>
     <t>Fuzhou, Yang Fuqing City, Fujian province</t>
   </si>
   <si>
@@ -1059,12 +1041,6 @@
     <t xml:space="preserve">#128 - Man,58, onset date April 21, hospitalized April 28 Cangshan District, Fuzhou, Fujian province </t>
   </si>
   <si>
-    <t>Wugang,</t>
-  </si>
-  <si>
-    <t>Shaoyang,</t>
-  </si>
-  <si>
     <t>Wugang, Shaoyang, Hunan province</t>
   </si>
   <si>
@@ -1116,9 +1092,6 @@
     <t>http://www.who.int/csr/don/2013_05_29/en/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Shaoxing </t>
-  </si>
-  <si>
     <t>hospitalized in critical condition</t>
   </si>
   <si>
@@ -1213,6 +1186,45 @@
   </si>
   <si>
     <t>http://news.xinhuanet.com/english/china/2013-12/18/c_132978520.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhejiang </t>
+  </si>
+  <si>
+    <t>Zhuji</t>
+  </si>
+  <si>
+    <t>A human case of H7N9 was reported in east China's Zhejiang Province on Sunday, the provincial health and family planning commission said in a statement. The patient is a 34-year-old woman surnamed Cai, who is from the city of Zhuji. She was confirmed to be infected with the bird flu virus on Saturday. By 1 p.m. on Sunday, she was still in critical condition at a local hospital, the statement said.</t>
+  </si>
+  <si>
+    <t>http://news.xinhuanet.com/english/china/2014-01/05/c_133020025.htm?utm_source=dlvr.it&amp;utm_medium=gplus</t>
+  </si>
+  <si>
+    <t>Patients Zhou Moumou, male, 86 years old, city residence, confirmed on Jan. 3, the city is now a hospital for treatment.</t>
+  </si>
+  <si>
+    <t>http://crofsblogs.typepad.com/h5n1/2014/01/china-shanghai-responds-to-the-new-h7n9-case.html?utm_source=dlvr.it&amp;utm_medium=gplus</t>
+  </si>
+  <si>
+    <t>Changzhou</t>
+  </si>
+  <si>
+    <t>Fuzhou</t>
+  </si>
+  <si>
+    <t>Wugang</t>
+  </si>
+  <si>
+    <t>Shaoxing</t>
+  </si>
+  <si>
+    <t>Xinyi</t>
+  </si>
+  <si>
+    <t>Xuzhou</t>
+  </si>
+  <si>
+    <t>Fuqing</t>
   </si>
 </sst>
 </file>
@@ -1271,8 +1283,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1364,7 +1402,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1406,6 +1444,19 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1447,6 +1498,19 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1776,12 +1840,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S151"/>
+  <dimension ref="A1:S153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="L150" sqref="L150"/>
+      <selection pane="bottomLeft" activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1794,7 +1858,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1818,28 +1882,28 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="L1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="O1" t="s">
         <v>9</v>
       </c>
       <c r="P1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="Q1" t="s">
         <v>10</v>
@@ -2131,7 +2195,7 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>46</v>
@@ -5944,7 +6008,7 @@
         <v>28</v>
       </c>
       <c r="E111" t="s">
-        <v>291</v>
+        <v>37</v>
       </c>
       <c r="H111" s="1">
         <v>39914</v>
@@ -5956,10 +6020,10 @@
         <v>199</v>
       </c>
       <c r="R111" t="s">
+        <v>291</v>
+      </c>
+      <c r="S111" t="s">
         <v>292</v>
-      </c>
-      <c r="S111" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:19">
@@ -5973,19 +6037,19 @@
         <v>69</v>
       </c>
       <c r="D112" t="s">
+        <v>293</v>
+      </c>
+      <c r="E112" t="s">
         <v>294</v>
-      </c>
-      <c r="E112" t="s">
-        <v>295</v>
       </c>
       <c r="H112" s="1">
         <v>39919</v>
       </c>
       <c r="Q112" t="s">
+        <v>295</v>
+      </c>
+      <c r="S112" t="s">
         <v>296</v>
-      </c>
-      <c r="S112" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="113" spans="1:19">
@@ -6002,19 +6066,19 @@
         <v>151</v>
       </c>
       <c r="E113" t="s">
+        <v>297</v>
+      </c>
+      <c r="F113" t="s">
         <v>298</v>
-      </c>
-      <c r="F113" t="s">
-        <v>299</v>
       </c>
       <c r="H113" s="1">
         <v>39919</v>
       </c>
       <c r="Q113" t="s">
+        <v>299</v>
+      </c>
+      <c r="S113" t="s">
         <v>300</v>
-      </c>
-      <c r="S113" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="114" spans="1:19">
@@ -6031,19 +6095,19 @@
         <v>45</v>
       </c>
       <c r="E114" t="s">
-        <v>302</v>
+        <v>55</v>
       </c>
       <c r="H114" s="1">
         <v>39919</v>
       </c>
       <c r="Q114" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="R114" t="s">
         <v>57</v>
       </c>
       <c r="S114" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="115" spans="1:19">
@@ -6060,19 +6124,19 @@
         <v>45</v>
       </c>
       <c r="E115" t="s">
-        <v>305</v>
+        <v>398</v>
       </c>
       <c r="H115" s="1">
         <v>39920</v>
       </c>
       <c r="Q115" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="R115" t="s">
         <v>57</v>
       </c>
       <c r="S115" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="116" spans="1:19">
@@ -6089,19 +6153,19 @@
         <v>45</v>
       </c>
       <c r="E116" t="s">
-        <v>302</v>
+        <v>55</v>
       </c>
       <c r="H116" s="1">
         <v>39919</v>
       </c>
       <c r="Q116" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="R116" t="s">
         <v>57</v>
       </c>
       <c r="S116" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:19">
@@ -6115,10 +6179,10 @@
         <v>65</v>
       </c>
       <c r="D117" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E117" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H117" s="1">
         <v>39920</v>
@@ -6127,10 +6191,10 @@
         <v>39925</v>
       </c>
       <c r="Q117" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="S117" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="118" spans="1:19">
@@ -6147,16 +6211,19 @@
         <v>28</v>
       </c>
       <c r="E118" t="s">
-        <v>313</v>
+        <v>25</v>
+      </c>
+      <c r="F118" t="s">
+        <v>310</v>
       </c>
       <c r="H118" s="1">
         <v>39919</v>
       </c>
       <c r="Q118" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="S118" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="119" spans="1:19">
@@ -6173,16 +6240,19 @@
         <v>28</v>
       </c>
       <c r="E119" t="s">
-        <v>316</v>
+        <v>400</v>
+      </c>
+      <c r="F119" t="s">
+        <v>399</v>
       </c>
       <c r="H119" s="1">
         <v>39921</v>
       </c>
       <c r="Q119" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="S119" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="120" spans="1:19">
@@ -6199,13 +6269,16 @@
         <v>28</v>
       </c>
       <c r="E120" t="s">
+        <v>41</v>
+      </c>
+      <c r="F120" t="s">
         <v>42</v>
       </c>
       <c r="Q120" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="S120" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="121" spans="1:19">
@@ -6219,19 +6292,19 @@
         <v>76</v>
       </c>
       <c r="D121" t="s">
+        <v>293</v>
+      </c>
+      <c r="E121" t="s">
         <v>294</v>
-      </c>
-      <c r="E121" t="s">
-        <v>295</v>
       </c>
       <c r="H121" s="1">
         <v>39919</v>
       </c>
       <c r="Q121" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="S121" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="122" spans="1:19">
@@ -6248,16 +6321,16 @@
         <v>215</v>
       </c>
       <c r="E122" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="H122" s="1">
         <v>39916</v>
       </c>
       <c r="Q122" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="S122" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="123" spans="1:19">
@@ -6271,13 +6344,13 @@
         <v>54</v>
       </c>
       <c r="D123" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E123" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F123" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H123" s="1">
         <v>39917</v>
@@ -6289,13 +6362,13 @@
         <v>7</v>
       </c>
       <c r="Q123" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="R123" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="S123" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:19">
@@ -6309,22 +6382,22 @@
         <v>80</v>
       </c>
       <c r="D124" t="s">
+        <v>293</v>
+      </c>
+      <c r="E124" t="s">
         <v>294</v>
-      </c>
-      <c r="E124" t="s">
-        <v>295</v>
       </c>
       <c r="H124" s="1">
         <v>39923</v>
       </c>
       <c r="Q124" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="R124" t="s">
         <v>57</v>
       </c>
       <c r="S124" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="125" spans="1:19">
@@ -6338,19 +6411,19 @@
         <v>31</v>
       </c>
       <c r="D125" t="s">
+        <v>293</v>
+      </c>
+      <c r="E125" t="s">
         <v>294</v>
-      </c>
-      <c r="E125" t="s">
-        <v>295</v>
       </c>
       <c r="H125" s="1">
         <v>39925</v>
       </c>
       <c r="Q125" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="S125" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="126" spans="1:19">
@@ -6373,13 +6446,13 @@
         <v>39920</v>
       </c>
       <c r="Q126" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="R126" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="S126" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="127" spans="1:19">
@@ -6393,25 +6466,25 @@
         <v>80</v>
       </c>
       <c r="D127" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E127" t="s">
-        <v>336</v>
+        <v>401</v>
       </c>
       <c r="F127" t="s">
-        <v>337</v>
+        <v>396</v>
       </c>
       <c r="I127" s="1">
         <v>39929</v>
       </c>
       <c r="Q127" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="R127" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="S127" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" spans="1:19">
@@ -6434,10 +6507,10 @@
         <v>39929</v>
       </c>
       <c r="Q128" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="S128" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" spans="1:19">
@@ -6451,13 +6524,13 @@
         <v>58</v>
       </c>
       <c r="D129" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E129" t="s">
+        <v>396</v>
+      </c>
+      <c r="F129" t="s">
         <v>337</v>
-      </c>
-      <c r="F129" t="s">
-        <v>343</v>
       </c>
       <c r="H129" s="1">
         <v>39923</v>
@@ -6466,10 +6539,10 @@
         <v>39930</v>
       </c>
       <c r="Q129" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="S129" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="130" spans="1:19">
@@ -6486,10 +6559,10 @@
         <v>215</v>
       </c>
       <c r="E130" t="s">
-        <v>346</v>
+        <v>397</v>
       </c>
       <c r="F130" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
       <c r="H130" s="1">
         <v>39925</v>
@@ -6498,13 +6571,13 @@
         <v>39929</v>
       </c>
       <c r="Q130" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="R130" t="s">
         <v>57</v>
       </c>
       <c r="S130" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="131" spans="1:19">
@@ -6582,7 +6655,7 @@
         <v>39915</v>
       </c>
       <c r="L133" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="134" spans="1:19">
@@ -6602,10 +6675,10 @@
         <v>14</v>
       </c>
       <c r="F134" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="G134" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H134" s="1">
         <v>39887</v>
@@ -6637,7 +6710,7 @@
         <v>39953</v>
       </c>
       <c r="O135" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="136" spans="1:19">
@@ -6663,7 +6736,7 @@
         <v>39994</v>
       </c>
       <c r="O136" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="137" spans="1:19">
@@ -6677,10 +6750,10 @@
         <v>61</v>
       </c>
       <c r="D137" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E137" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G137" t="s">
         <v>132</v>
@@ -6698,7 +6771,7 @@
         <v>40013</v>
       </c>
       <c r="O137" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="138" spans="1:19">
@@ -6712,7 +6785,7 @@
         <v>51</v>
       </c>
       <c r="D138" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E138" t="s">
         <v>105</v>
@@ -6730,16 +6803,16 @@
         <v>40033</v>
       </c>
       <c r="L138" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="N138" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="O138" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="P138" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="139" spans="1:19">
@@ -6756,7 +6829,7 @@
         <v>45</v>
       </c>
       <c r="E139" t="s">
-        <v>365</v>
+        <v>398</v>
       </c>
       <c r="H139" s="1">
         <v>40093</v>
@@ -6768,10 +6841,10 @@
         <v>40100</v>
       </c>
       <c r="L139" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="O139" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="140" spans="1:19">
@@ -6794,10 +6867,10 @@
         <v>40101</v>
       </c>
       <c r="L140" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="O140" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="141" spans="1:19">
@@ -6811,10 +6884,10 @@
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E141" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="H141" s="1">
         <v>40114</v>
@@ -6826,13 +6899,13 @@
         <v>40121</v>
       </c>
       <c r="L141" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="O141" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="P141" s="2" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="142" spans="1:19">
@@ -6858,10 +6931,10 @@
         <v>40121</v>
       </c>
       <c r="L142" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="O142" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="143" spans="1:19">
@@ -6881,7 +6954,7 @@
         <v>52</v>
       </c>
       <c r="F143" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="G143" t="s">
         <v>45</v>
@@ -6896,10 +6969,10 @@
         <v>40144</v>
       </c>
       <c r="L143" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="O143" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="144" spans="1:19">
@@ -6913,13 +6986,13 @@
         <v>36</v>
       </c>
       <c r="D144" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="E144" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="G144" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="H144" s="1">
         <v>40137</v>
@@ -6931,10 +7004,10 @@
         <v>40149</v>
       </c>
       <c r="L144" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="O144" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="145" spans="1:16" ht="15" customHeight="1">
@@ -6948,13 +7021,13 @@
         <v>80</v>
       </c>
       <c r="D145" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="E145" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="G145" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="H145" s="1">
         <v>40149</v>
@@ -6969,7 +7042,7 @@
         <v>40152</v>
       </c>
       <c r="L145" s="3" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="M145" t="b">
         <v>1</v>
@@ -6978,10 +7051,10 @@
         <v>7</v>
       </c>
       <c r="O145" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="P145" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="146" spans="1:16" ht="15" customHeight="1">
@@ -7001,7 +7074,7 @@
         <v>52</v>
       </c>
       <c r="F146" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="H146" s="1">
         <v>40145</v>
@@ -7013,10 +7086,10 @@
         <v>40151</v>
       </c>
       <c r="L146" s="3" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="O146" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="147" spans="1:16">
@@ -7030,10 +7103,10 @@
         <v>39</v>
       </c>
       <c r="D147" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E147" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="H147" s="1">
         <v>40152</v>
@@ -7042,10 +7115,10 @@
         <v>40160</v>
       </c>
       <c r="L147" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="O147" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="148" spans="1:16">
@@ -7059,16 +7132,16 @@
         <v>65</v>
       </c>
       <c r="D148" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E148" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="K148" s="1">
         <v>40162</v>
       </c>
       <c r="O148" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="149" spans="1:16">
@@ -7082,13 +7155,13 @@
         <v>38</v>
       </c>
       <c r="D149" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E149" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="F149" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="H149" s="1">
         <v>40155</v>
@@ -7097,7 +7170,7 @@
         <v>40165</v>
       </c>
       <c r="O149" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="150" spans="1:16">
@@ -7111,16 +7184,16 @@
         <v>62</v>
       </c>
       <c r="D150" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E150" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="K150" s="1">
         <v>40164</v>
       </c>
       <c r="O150" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="151" spans="1:16" ht="15" customHeight="1">
@@ -7136,8 +7209,11 @@
       <c r="D151" t="s">
         <v>28</v>
       </c>
+      <c r="E151" t="s">
+        <v>395</v>
+      </c>
       <c r="G151" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="H151" s="1">
         <v>40165</v>
@@ -7149,10 +7225,65 @@
         <v>40177</v>
       </c>
       <c r="L151" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="O151" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>13</v>
+      </c>
+      <c r="C152">
+        <v>86</v>
+      </c>
+      <c r="D152" t="s">
+        <v>14</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="I152" s="1">
+        <v>39815</v>
+      </c>
+      <c r="K152" s="1">
+        <v>39816</v>
+      </c>
+      <c r="L152" t="s">
         <v>393</v>
       </c>
-      <c r="O151" t="s">
+      <c r="O152" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>22</v>
+      </c>
+      <c r="C153">
+        <v>34</v>
+      </c>
+      <c r="D153" t="s">
+        <v>389</v>
+      </c>
+      <c r="E153" t="s">
+        <v>390</v>
+      </c>
+      <c r="K153" s="1">
+        <v>40182</v>
+      </c>
+      <c r="L153" t="s">
+        <v>391</v>
+      </c>
+      <c r="O153" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 new cases and some updated dates and references
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="407">
   <si>
     <t>gender</t>
   </si>
@@ -1197,15 +1197,9 @@
     <t>A human case of H7N9 was reported in east China's Zhejiang Province on Sunday, the provincial health and family planning commission said in a statement. The patient is a 34-year-old woman surnamed Cai, who is from the city of Zhuji. She was confirmed to be infected with the bird flu virus on Saturday. By 1 p.m. on Sunday, she was still in critical condition at a local hospital, the statement said.</t>
   </si>
   <si>
-    <t>http://news.xinhuanet.com/english/china/2014-01/05/c_133020025.htm?utm_source=dlvr.it&amp;utm_medium=gplus</t>
-  </si>
-  <si>
     <t>Patients Zhou Moumou, male, 86 years old, city residence, confirmed on Jan. 3, the city is now a hospital for treatment.</t>
   </si>
   <si>
-    <t>http://crofsblogs.typepad.com/h5n1/2014/01/china-shanghai-responds-to-the-new-h7n9-case.html?utm_source=dlvr.it&amp;utm_medium=gplus</t>
-  </si>
-  <si>
     <t>Changzhou</t>
   </si>
   <si>
@@ -1225,6 +1219,27 @@
   </si>
   <si>
     <t>Fuqing</t>
+  </si>
+  <si>
+    <t>Foshan</t>
+  </si>
+  <si>
+    <t>The CHP said today that one of the patients is a 47-year-old man who is a poultry worker from Foshan and became ill on Dec 25. He was hospitalized in Guangzhou on Jan 3 and is in critical condition. Provincial health officials are monitoring 60 of the man’s close contacts, but no far no other H7N9 infections have been detected.</t>
+  </si>
+  <si>
+    <t>Guangdong province’s other new case involves a 71-year-old man from Yangjiang who got sick on Jan 1 and was admitted to a hospital on Jan 4 where he is in critical condition, according to the CHP. He had no history of recent contact with poultry. Authorities have 65 of his close contacts under medical surveillance, but so far no other cases have been found.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_01_06/en/index.html</t>
+  </si>
+  <si>
+    <t>http://www.chp.gov.hk/en/content/116/32906.html</t>
+  </si>
+  <si>
+    <t>http://www.chp.gov.hk/en/content/116/32886.html</t>
+  </si>
+  <si>
+    <t>http://www.chp.gov.hk/en/content/116/32884.html</t>
   </si>
 </sst>
 </file>
@@ -1283,8 +1298,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1402,7 +1423,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1457,6 +1478,9 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1511,6 +1535,9 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1840,12 +1867,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S153"/>
+  <dimension ref="A1:S155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="E139" sqref="E139"/>
+      <selection pane="bottomLeft" activeCell="N157" sqref="N157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6124,7 +6151,7 @@
         <v>45</v>
       </c>
       <c r="E115" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H115" s="1">
         <v>39920</v>
@@ -6240,10 +6267,10 @@
         <v>28</v>
       </c>
       <c r="E119" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F119" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H119" s="1">
         <v>39921</v>
@@ -6469,10 +6496,10 @@
         <v>306</v>
       </c>
       <c r="E127" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F127" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I127" s="1">
         <v>39929</v>
@@ -6527,7 +6554,7 @@
         <v>306</v>
       </c>
       <c r="E129" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F129" t="s">
         <v>337</v>
@@ -6559,7 +6586,7 @@
         <v>215</v>
       </c>
       <c r="E130" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F130" t="s">
         <v>319</v>
@@ -6829,7 +6856,7 @@
         <v>45</v>
       </c>
       <c r="E139" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H139" s="1">
         <v>40093</v>
@@ -7166,11 +7193,17 @@
       <c r="H149" s="1">
         <v>40155</v>
       </c>
+      <c r="I149" s="1">
+        <v>40164</v>
+      </c>
       <c r="K149" s="1">
         <v>40165</v>
       </c>
       <c r="O149" t="s">
         <v>382</v>
+      </c>
+      <c r="P149" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="1:16">
@@ -7189,11 +7222,20 @@
       <c r="E150" t="s">
         <v>379</v>
       </c>
+      <c r="H150" s="1">
+        <v>40157</v>
+      </c>
+      <c r="I150" s="1">
+        <v>40162</v>
+      </c>
       <c r="K150" s="1">
         <v>40164</v>
       </c>
       <c r="O150" t="s">
         <v>388</v>
+      </c>
+      <c r="P150" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="151" spans="1:16" ht="15" customHeight="1">
@@ -7210,7 +7252,7 @@
         <v>28</v>
       </c>
       <c r="E151" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G151" t="s">
         <v>383</v>
@@ -7254,10 +7296,10 @@
         <v>39816</v>
       </c>
       <c r="L152" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="O152" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
     </row>
     <row r="153" spans="1:16">
@@ -7276,6 +7318,12 @@
       <c r="E153" t="s">
         <v>390</v>
       </c>
+      <c r="H153" s="1">
+        <v>40175</v>
+      </c>
+      <c r="I153" s="1">
+        <v>40179</v>
+      </c>
       <c r="K153" s="1">
         <v>40182</v>
       </c>
@@ -7283,7 +7331,71 @@
         <v>391</v>
       </c>
       <c r="O153" t="s">
-        <v>392</v>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>13</v>
+      </c>
+      <c r="C154">
+        <v>47</v>
+      </c>
+      <c r="D154" t="s">
+        <v>345</v>
+      </c>
+      <c r="E154" t="s">
+        <v>400</v>
+      </c>
+      <c r="H154" s="1">
+        <v>40171</v>
+      </c>
+      <c r="I154" s="1">
+        <v>40180</v>
+      </c>
+      <c r="K154" s="1">
+        <v>40184</v>
+      </c>
+      <c r="L154" t="s">
+        <v>401</v>
+      </c>
+      <c r="O154" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>13</v>
+      </c>
+      <c r="C155">
+        <v>71</v>
+      </c>
+      <c r="D155" t="s">
+        <v>345</v>
+      </c>
+      <c r="E155" t="s">
+        <v>379</v>
+      </c>
+      <c r="H155" s="1">
+        <v>40178</v>
+      </c>
+      <c r="I155" s="1">
+        <v>40181</v>
+      </c>
+      <c r="K155" s="1">
+        <v>40184</v>
+      </c>
+      <c r="L155" t="s">
+        <v>402</v>
+      </c>
+      <c r="O155" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added date of death for latest case
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17640" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -2039,7 +2039,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A85" sqref="A85"/>
-      <selection pane="bottomLeft" activeCell="A156" sqref="A156:XFD156"/>
+      <selection pane="bottomLeft" activeCell="K166" sqref="K166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7925,6 +7925,9 @@
       <c r="I166" s="1">
         <v>40185</v>
       </c>
+      <c r="J166" s="1">
+        <v>40187</v>
+      </c>
       <c r="K166" s="1">
         <v>40190</v>
       </c>

</xml_diff>

<commit_message>
Added 62 new cases from the last couple of weeks.
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="39980" windowHeight="25700" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="575">
   <si>
     <t>gender</t>
   </si>
@@ -1501,6 +1501,249 @@
   </si>
   <si>
     <t>A 63 year old woman from Taizhou City, Zhejiang Province, who became ill on 9 January. He was admitted to hospital on 13 January, transferred to another hospital on 18 January, and is in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>Changping</t>
+  </si>
+  <si>
+    <t>A 58 year old man from Changping District, Beijing, who became ill on 12 January. He was admitted to hospital on 16 January and transferred to another hospital on 24 January. He is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/entity/csr/don/2014_01_25/en/index.html</t>
+  </si>
+  <si>
+    <t>A 78 year old woman from Ningbo City,Zhejiang Province, who became ill on 17 January. She was admitted to hospital on 20 January and transferred to another hospital on 23 January. She is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 44 year old woman from Ningbo City, Zhejiang Province, who became ill on 17 January. She was admitted to hospital on 20 January and is currently in a serious condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 23 year old woman from Hangzhou City, Zhejiang Province, who became ill on 20 January. She was admitted to hospital on 22 January and is currently in a serious condition. The patient has a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>A 82 year old woman from Hangzhou City, Zhejiang Province, who became ill on 16 January. She was admitted to hospital on 17 January and is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 73 year old man from Shaoxing City, Zhejiang Province, who became ill on 18 January. He was admitted to hospital on 21 January and is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 62 year old woman farmer from Shaoxing City, Zhejiang Province, who became ill on 15 January. She was admitted to hospital on 20 January and transferred to another hospital on 21 January. She is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 33 year old farmer from Shaoxing City, Zhejiang Province, who became ill on 17 January. He was admitted to hospital on 19 January and is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 58 year old woman from Huizhou City, Guangdong Province, who became ill on 10 January. She was admitted to hospital on 16 January and transferred to another hospital on 23 January. She is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>Meizhou</t>
+  </si>
+  <si>
+    <t>A 52 year old poultry salesman from Meizhou City, Guangdong Province, who became ill on 14 January. He was admitted to hospital on 20 January and is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 49 year old man from Huzhou City, Zhejiang Province, who became ill on 16 January. He was admitted to hospital on 20 January and transferred to other hospital on 23 January. He is currently in a serious condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_01_27/en/index.html</t>
+  </si>
+  <si>
+    <t>A 60 year old woman farmer from Ningbo City, Zhejiang Province, who became ill on 19 January. She was admitted to hospital on 23 January. She is currently in a serious condition.</t>
+  </si>
+  <si>
+    <t>A 48 year old woman farmer from Ningbo City, Zhejiang Province, who became ill on 20 January. She was admitted to hospital on 23 January and is currently in a serious condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 57 year old farmer from Suzhou City, Jiangsu Province, who became ill on 16 January. He was admitted to hospital on 19 January and transferred to other hospital on 22 January. He is currently in a serious condition. The patient has a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>A 46 year old woman farmer from Quanzhou City, Fujian Province, who became ill on 18 January. She was admitted to hospital on 22 January and is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 82 year old man from Shenzhen City, Guangdong Province, who became ill on 11 January. He was admitted to hospital on 21 January and is currently in a critical condition. The patient has a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>A 76 year-old farmer from Wuxi City, Jiangsu Province, who became ill on 18 January. He was admitted to hospital on 21 January and is currently in a serious condition.</t>
+  </si>
+  <si>
+    <t>A 40 year-old man from Hangzhou City, Zhejiang Province, who became ill on 19 January. He was admitted to hospital on 23 January and was transferred to another hospital on 25 January. He is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 65 year-old, man from Huzhou City, Zhejiang Province, who became ill on 16 January. He was admitted to hospital on 22 January and was transferred to another hospital on 23 January. He is currently in a serious condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 74-year-old woman farmer from Suzhou City, Jiangsu Province, who became ill on 15 January. She was admitted to hospital on 21 January 2014, and was transferred to another hospital on 24 January. She is currently in critical condition and is being given intensive treatment. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_01_29/en/index.html</t>
+  </si>
+  <si>
+    <t>Yueyang</t>
+  </si>
+  <si>
+    <t>A 58-year-old woman farmer from Yueyang City, Hunan Province, who became ill on 20 January. She was admitted to hospital on 25 January. She is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>Xiamen</t>
+  </si>
+  <si>
+    <t>A 69-year-old man from Xiamen City, Fujian Province, who became ill on 17 January. He was admitted to hospital on 24 January. He is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>Sanming</t>
+  </si>
+  <si>
+    <t>A 72-year-old woman farmer from Sanming City, Fujian Province, who became ill on 21 January. She was admitted to hospital on 23 January. She is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 77-year-old woman farmer, from Shenzhen City, Guangdong Province, who became ill in 17 January. She was admitted to hospital on 23 January. She is currently in a critical condition. The patient has a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>Jiangmen</t>
+  </si>
+  <si>
+    <t>A 68-year-old farmer from Jiangmen City, Guangdong Province, who became ill on 18 January. He was admitted to hospital on 21 January. He died on 25 January. The patient had a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 61-year-old woman cook from Shanghai City who became ill on 6 January. She was admitted to hospital on 20 January. She is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_01_30/en/index.html</t>
+  </si>
+  <si>
+    <t>A 66-year-old woman from Shaoxing City, Zhejiang Province, who became ill on 15 January. She was admitted to hospital on 17 January. She is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 71-year-old woman from Hangzhou City, Zhejiang Province, who became ill on 12 January. She was admitted to hospital on 18 January. She is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 71-year- old farmer from Wenzhou City, Zhejiang Province, who became ill on 13 January. He was admitted to hospital on 19 January, and was transferred to another hospital on 21 January 2014. He is currently in a serious condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 59-year- old man from Ningbo City, Zhejiang Province, who became ill on 18 January. He was admitted to hospital on 20 January and was transferred to another hospital on 22 January. He is currently in a serious condition. He has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 63-years-old woman farmer from Huzhou City, Zhejiang Province, who became ill on 11 January. She was admitted to hospital on 15 January and was transferred to another hospital on 18 January 2014. She is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 34-year- old woman from Shenzhen City, Guangdong Province, who became ill on 10 January. She was admitted to hospital on 20 January 2014, and was transferred to another hospital on 21 January 2014. She is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>Huai'an</t>
+  </si>
+  <si>
+    <t>A 53-year- old man from Huai'an City, Jiangsu Province, who became ill on 22 January. He was admitted to hospital on 26 January. He is currently in a serious condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 43-year-old woman farmer from Hangzhou City, Zhejiang Province, who became ill on 23 January. She was admitted to hospital on the same day. She has a mild illness. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>An 81-year-old farmer from Huzhou City, Zhejiang Province, who became ill on 21 January. He was admitted to hospital on 23 January. He is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 63-year-old woman farmer from Huzhou City, Zhejiang Province, who became ill on 22 January. She was admitted to hospital on 24 January and was transferred to another hospital on 26 January 2014. She is currently in a serious condition. The patient has a history of exposure to a live poultry environment.</t>
+  </si>
+  <si>
+    <t>A 57-year-old man from Ningbo City, Zhejiang Province, who became ill on 15 January. He was admitted to hospital on 23 January. He has a mild illness. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 43-year-old woman from Shenzhen City, Guangdong Province, who became ill on 17 January. She was admitted to hospital on 26 January. She is currently in a serious condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 41-year-old woman from Shenzhen City, Guangdong Province, who became ill on 20 January. She was admitted to hospital on 26 January. She is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 31-year-old woman from Shenzhen City, Guangdong Province, who became ill on 16 January. She was admitted to hospital on 23 January 2014. She is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 37-year-old farmer from Wenzhou City, Zhejiang Province, who became ill on 19 January. He was admitted to hospital on 27 January and was transferred to another hospital on 28 January. He is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_01_31/en/index.html</t>
+  </si>
+  <si>
+    <t>A 60-year-old man from Hangzhou City, Zhejiang Province, who became ill on 23 January. He was admitted to hospital on 28 January and is currently in a serious condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 63-year-old man from Hangzhou City, Zhejiang Province, who became ill on 24 January. He was admitted to hospital on 27 January and is currently in a serious condition. He has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 2-year-and-8-month old boy from Xiamen City, Fujian Province, who became ill on 26 January. He was admitted to hospital on 28 January and has a mild illness. His family slaughter and sell ducks.</t>
+  </si>
+  <si>
+    <t>A 17-year-old man from Guangzhou City, Guangdong Province, who became ill on 22 January. He was admitted to hospital on 27 January and is currently in a serious condition.</t>
+  </si>
+  <si>
+    <t>A 75-year-old man with underlying illnesses who travelled alone to Shenzhen between 20 to 26 January became ill while in Shenzhen on 26 January. He was admitted to hospital in Hong Kong on 28 January and died on 29 January. During his stay in Shenzhen it is reported that he stayed with relatives who lived close to a live poultry market. His five home contacts in Hong Kong have remained asymptomatic but have been admitted to hospital for observation. Further investigations into the man’s travel and exposure histories are ongoing, in parallel with tracing of other contacts of the case, including four patients with whom he shared a hospital room, and healthcare and ambulance staff. Preliminary findings suggest that the man was infected outside of Hong Kong SAR.</t>
+  </si>
+  <si>
+    <t>A 75-year-old farmer from Ningpo City, Zhejiang Province, who became ill on 21 January and was admitted to hospital on 24 January. He is currently in a critical condition The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_01/en/index.html</t>
+  </si>
+  <si>
+    <t>A 76 year-old man from Ningpo City, Zhejiang Province, who became ill on 21 January 2014 and was admitted to hospital on 24 January and transferred to another hospital on 27 January. He is currently in a critical condition. He has a history of exposure to a poultry market.</t>
+  </si>
+  <si>
+    <t>A 78-year-old farmer from Hangzhou City, Zhejiang Province, who became ill on 25 January and was admitted to hospital on 27 January and transferred to another hospital on 29 January. He is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 64-year-old man from Ningpo City, Zhejiang Province, who became ill on 13 January and was admitted to hospital on 16 January. He is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 75-year-old woman from Nanjing City, Jiangsu Province, who became ill on 18 January and was admitted to hospital on 25 January. She is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 67-year-old woman from Jiangmen City, Guangdong Province, who became ill on 24 January and was admitted to hospital on 25 January. She died on 28 January 2014. The patient had a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>Guangxi</t>
+  </si>
+  <si>
+    <t>Hezhou</t>
+  </si>
+  <si>
+    <t>A 56 year-old woman from Hezhou City, Guangxi Province, who became ill on 20 January and was admitted to hospital on 27 January. She is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 80-year-old man from Hangzhou City, Zhejiang Province, who became ill on 19 January and was admitted to hospital on 30 January. He is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_03/en/index.html</t>
+  </si>
+  <si>
+    <t>A 54-year-old man from Hangzhou City, Zhejiang Province, who became ill on 23 January and was admitted to hospital on 26 January. He is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 6-year-old boy who is living in Shenzhen City, Guangdong Province, and became ill on 27 January. He was detected on 28 January by Shenzhen Entry-Exit Quarantine Bureau when travelling through Huanggang Port. He has mild symptoms and is in a stable condition. He is currently in isolated treatment at home. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>Zhaoqing</t>
+  </si>
+  <si>
+    <t>A 5-year old boy from Zhaoqing City, Guangdong Province, who became ill on 29 January and admitted to hospital on the same day. He is in a stable condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 28-year-old man from Zhaoqing City, Guangdong Province, who became ill on 24 January 2014 and admitted to hospital on 26 January. He is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 82-year-old man from Foshan City, Guangdong Province, who became ill on 22 January and admitted to hospital on 26 January. He is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 59-year-old man from Guangzhou City, Guangdong Province, who became ill on 22 January and admitted to hospital on 26 January. He died on 30 January. The patient had a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 81-year-old woman from Shenzhen City, Guangdong Province, who became ill on 25 January and admitted to hospital on 29 January. She is currently in a serious condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>Yongzhou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2014-01-24</t>
+  </si>
+  <si>
+    <t>A 38-year-old male from Yongzhou City, Hunan Province with onset of symptoms on 24 January 2014. He was admitted to hospital on 30 January and is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1842,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="351">
+  <cellStyleXfs count="365">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1951,8 +2194,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1966,8 +2223,9 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="351">
+  <cellStyles count="365">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2143,6 +2401,13 @@
     <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2318,6 +2583,13 @@
     <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -2339,8 +2611,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S222" totalsRowShown="0">
-  <autoFilter ref="A1:S222"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S284" totalsRowShown="0">
+  <autoFilter ref="A1:S284"/>
   <tableColumns count="19">
     <tableColumn id="1" name="number"/>
     <tableColumn id="2" name="gender"/>
@@ -2688,13 +2960,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S222"/>
+  <dimension ref="A1:S284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F253" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
+      <selection pane="bottomRight" activeCell="E272" sqref="E272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9973,7 +10245,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:19">
       <c r="A209">
         <v>208</v>
       </c>
@@ -10017,7 +10289,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="210" spans="1:16" s="9" customFormat="1">
+    <row r="210" spans="1:19" s="9" customFormat="1">
       <c r="A210">
         <v>209</v>
       </c>
@@ -10050,7 +10322,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="211" spans="1:16" s="9" customFormat="1">
+    <row r="211" spans="1:19" s="9" customFormat="1">
       <c r="A211">
         <v>210</v>
       </c>
@@ -10083,7 +10355,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="212" spans="1:16" s="9" customFormat="1">
+    <row r="212" spans="1:19" s="9" customFormat="1">
       <c r="A212">
         <v>211</v>
       </c>
@@ -10116,7 +10388,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="213" spans="1:16" s="9" customFormat="1">
+    <row r="213" spans="1:19" s="9" customFormat="1">
       <c r="A213">
         <v>212</v>
       </c>
@@ -10149,7 +10421,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="214" spans="1:16" s="9" customFormat="1">
+    <row r="214" spans="1:19" s="9" customFormat="1">
       <c r="A214">
         <v>213</v>
       </c>
@@ -10182,7 +10454,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="215" spans="1:16" s="9" customFormat="1">
+    <row r="215" spans="1:19" s="9" customFormat="1">
       <c r="A215">
         <v>214</v>
       </c>
@@ -10215,7 +10487,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="216" spans="1:16" s="9" customFormat="1">
+    <row r="216" spans="1:19" s="9" customFormat="1">
       <c r="A216">
         <v>215</v>
       </c>
@@ -10248,7 +10520,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="217" spans="1:16" s="9" customFormat="1">
+    <row r="217" spans="1:19" s="9" customFormat="1">
       <c r="A217">
         <v>216</v>
       </c>
@@ -10281,7 +10553,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="218" spans="1:16" s="9" customFormat="1">
+    <row r="218" spans="1:19" s="9" customFormat="1">
       <c r="A218">
         <v>217</v>
       </c>
@@ -10316,7 +10588,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="219" spans="1:16" s="9" customFormat="1">
+    <row r="219" spans="1:19" s="9" customFormat="1">
       <c r="A219">
         <v>218</v>
       </c>
@@ -10351,7 +10623,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="220" spans="1:16" s="9" customFormat="1">
+    <row r="220" spans="1:19" s="9" customFormat="1">
       <c r="A220">
         <v>219</v>
       </c>
@@ -10386,7 +10658,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="221" spans="1:16" s="9" customFormat="1">
+    <row r="221" spans="1:19" s="9" customFormat="1">
       <c r="A221">
         <v>220</v>
       </c>
@@ -10421,7 +10693,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="222" spans="1:16" s="9" customFormat="1">
+    <row r="222" spans="1:19" s="9" customFormat="1">
       <c r="A222">
         <v>221</v>
       </c>
@@ -10455,6 +10727,2268 @@
       <c r="O222" s="7" t="s">
         <v>483</v>
       </c>
+    </row>
+    <row r="223" spans="1:19">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223" t="s">
+        <v>13</v>
+      </c>
+      <c r="C223">
+        <v>58</v>
+      </c>
+      <c r="D223" t="s">
+        <v>132</v>
+      </c>
+      <c r="E223" t="s">
+        <v>132</v>
+      </c>
+      <c r="F223" t="s">
+        <v>494</v>
+      </c>
+      <c r="H223" s="1">
+        <v>40189</v>
+      </c>
+      <c r="I223" s="1">
+        <v>40201</v>
+      </c>
+      <c r="K223" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L223" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="O223" t="s">
+        <v>496</v>
+      </c>
+      <c r="P223" s="9"/>
+      <c r="Q223" s="9"/>
+      <c r="R223" s="9"/>
+      <c r="S223" s="9"/>
+    </row>
+    <row r="224" spans="1:19">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224" t="s">
+        <v>22</v>
+      </c>
+      <c r="C224">
+        <v>78</v>
+      </c>
+      <c r="D224" t="s">
+        <v>45</v>
+      </c>
+      <c r="E224" t="s">
+        <v>408</v>
+      </c>
+      <c r="H224" s="1">
+        <v>40194</v>
+      </c>
+      <c r="I224" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K224" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L224" t="s">
+        <v>497</v>
+      </c>
+      <c r="O224" t="s">
+        <v>496</v>
+      </c>
+      <c r="P224" s="9"/>
+      <c r="Q224" s="9"/>
+      <c r="R224" s="9"/>
+      <c r="S224" s="9"/>
+    </row>
+    <row r="225" spans="1:19">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225" t="s">
+        <v>22</v>
+      </c>
+      <c r="C225">
+        <v>44</v>
+      </c>
+      <c r="D225" t="s">
+        <v>45</v>
+      </c>
+      <c r="E225" t="s">
+        <v>408</v>
+      </c>
+      <c r="H225" s="1">
+        <v>40194</v>
+      </c>
+      <c r="I225" s="1">
+        <v>40197</v>
+      </c>
+      <c r="K225" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L225" t="s">
+        <v>498</v>
+      </c>
+      <c r="O225" t="s">
+        <v>496</v>
+      </c>
+      <c r="P225" s="9"/>
+      <c r="Q225" s="9"/>
+      <c r="R225" s="9"/>
+      <c r="S225" s="9"/>
+    </row>
+    <row r="226" spans="1:19">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226" t="s">
+        <v>22</v>
+      </c>
+      <c r="C226">
+        <v>23</v>
+      </c>
+      <c r="D226" t="s">
+        <v>45</v>
+      </c>
+      <c r="E226" t="s">
+        <v>52</v>
+      </c>
+      <c r="H226" s="1">
+        <v>40197</v>
+      </c>
+      <c r="I226" s="1">
+        <v>40199</v>
+      </c>
+      <c r="K226" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L226" t="s">
+        <v>499</v>
+      </c>
+      <c r="O226" t="s">
+        <v>496</v>
+      </c>
+      <c r="P226" s="9"/>
+      <c r="Q226" s="9"/>
+      <c r="R226" s="9"/>
+      <c r="S226" s="9"/>
+    </row>
+    <row r="227" spans="1:19">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227" t="s">
+        <v>22</v>
+      </c>
+      <c r="C227">
+        <v>82</v>
+      </c>
+      <c r="D227" t="s">
+        <v>45</v>
+      </c>
+      <c r="E227" t="s">
+        <v>52</v>
+      </c>
+      <c r="H227" s="1">
+        <v>40193</v>
+      </c>
+      <c r="I227" s="1">
+        <v>40194</v>
+      </c>
+      <c r="K227" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L227" t="s">
+        <v>500</v>
+      </c>
+      <c r="O227" t="s">
+        <v>496</v>
+      </c>
+      <c r="P227" s="9"/>
+      <c r="Q227" s="9"/>
+      <c r="R227" s="9"/>
+      <c r="S227" s="9"/>
+    </row>
+    <row r="228" spans="1:19">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228" t="s">
+        <v>13</v>
+      </c>
+      <c r="C228">
+        <v>73</v>
+      </c>
+      <c r="D228" t="s">
+        <v>45</v>
+      </c>
+      <c r="E228" t="s">
+        <v>394</v>
+      </c>
+      <c r="H228" s="1">
+        <v>40195</v>
+      </c>
+      <c r="I228" s="1">
+        <v>40198</v>
+      </c>
+      <c r="K228" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L228" t="s">
+        <v>501</v>
+      </c>
+      <c r="O228" t="s">
+        <v>496</v>
+      </c>
+      <c r="P228" s="9"/>
+      <c r="Q228" s="9"/>
+      <c r="R228" s="9"/>
+      <c r="S228" s="9"/>
+    </row>
+    <row r="229" spans="1:19">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229" t="s">
+        <v>22</v>
+      </c>
+      <c r="C229">
+        <v>62</v>
+      </c>
+      <c r="D229" t="s">
+        <v>45</v>
+      </c>
+      <c r="E229" t="s">
+        <v>394</v>
+      </c>
+      <c r="H229" s="1">
+        <v>40192</v>
+      </c>
+      <c r="I229" s="1">
+        <v>40198</v>
+      </c>
+      <c r="K229" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L229" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="O229" t="s">
+        <v>496</v>
+      </c>
+      <c r="P229" s="9"/>
+      <c r="Q229" s="9"/>
+      <c r="R229" s="9"/>
+      <c r="S229" s="9"/>
+    </row>
+    <row r="230" spans="1:19">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230" t="s">
+        <v>13</v>
+      </c>
+      <c r="C230">
+        <v>33</v>
+      </c>
+      <c r="D230" t="s">
+        <v>45</v>
+      </c>
+      <c r="E230" t="s">
+        <v>394</v>
+      </c>
+      <c r="H230" s="1">
+        <v>40194</v>
+      </c>
+      <c r="I230" s="1">
+        <v>40196</v>
+      </c>
+      <c r="K230" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L230" t="s">
+        <v>503</v>
+      </c>
+      <c r="O230" t="s">
+        <v>496</v>
+      </c>
+      <c r="P230" s="9"/>
+      <c r="Q230" s="9"/>
+      <c r="R230" s="9"/>
+      <c r="S230" s="9"/>
+    </row>
+    <row r="231" spans="1:19">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231" t="s">
+        <v>22</v>
+      </c>
+      <c r="C231">
+        <v>58</v>
+      </c>
+      <c r="D231" t="s">
+        <v>345</v>
+      </c>
+      <c r="E231" t="s">
+        <v>105</v>
+      </c>
+      <c r="H231" s="1">
+        <v>40187</v>
+      </c>
+      <c r="I231" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K231" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L231" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="O231" t="s">
+        <v>496</v>
+      </c>
+      <c r="P231" s="9"/>
+      <c r="Q231" s="9"/>
+      <c r="R231" s="9"/>
+      <c r="S231" s="9"/>
+    </row>
+    <row r="232" spans="1:19">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232" t="s">
+        <v>13</v>
+      </c>
+      <c r="C232">
+        <v>52</v>
+      </c>
+      <c r="D232" t="s">
+        <v>345</v>
+      </c>
+      <c r="E232" t="s">
+        <v>505</v>
+      </c>
+      <c r="H232" s="1">
+        <v>40191</v>
+      </c>
+      <c r="I232" s="1">
+        <v>40197</v>
+      </c>
+      <c r="K232" s="1">
+        <v>40202</v>
+      </c>
+      <c r="L232" t="s">
+        <v>506</v>
+      </c>
+      <c r="O232" t="s">
+        <v>496</v>
+      </c>
+      <c r="P232" s="9"/>
+      <c r="Q232" s="9"/>
+      <c r="R232" s="9"/>
+      <c r="S232" s="9"/>
+    </row>
+    <row r="233" spans="1:19">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233" t="s">
+        <v>13</v>
+      </c>
+      <c r="C233">
+        <v>49</v>
+      </c>
+      <c r="D233" t="s">
+        <v>45</v>
+      </c>
+      <c r="E233" t="s">
+        <v>55</v>
+      </c>
+      <c r="H233" s="1">
+        <v>40193</v>
+      </c>
+      <c r="I233" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K233" s="1">
+        <v>40203</v>
+      </c>
+      <c r="L233" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="O233" t="s">
+        <v>508</v>
+      </c>
+      <c r="P233" s="9"/>
+      <c r="Q233" s="9"/>
+      <c r="R233" s="9"/>
+      <c r="S233" s="9"/>
+    </row>
+    <row r="234" spans="1:19">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>22</v>
+      </c>
+      <c r="C234">
+        <v>60</v>
+      </c>
+      <c r="D234" t="s">
+        <v>45</v>
+      </c>
+      <c r="E234" t="s">
+        <v>408</v>
+      </c>
+      <c r="H234" s="1">
+        <v>40196</v>
+      </c>
+      <c r="I234" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K234" s="1">
+        <v>40203</v>
+      </c>
+      <c r="L234" t="s">
+        <v>509</v>
+      </c>
+      <c r="O234" t="s">
+        <v>508</v>
+      </c>
+      <c r="P234" s="9"/>
+      <c r="Q234" s="9"/>
+      <c r="R234" s="9"/>
+      <c r="S234" s="9"/>
+    </row>
+    <row r="235" spans="1:19">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" t="s">
+        <v>22</v>
+      </c>
+      <c r="C235">
+        <v>48</v>
+      </c>
+      <c r="D235" t="s">
+        <v>45</v>
+      </c>
+      <c r="E235" t="s">
+        <v>408</v>
+      </c>
+      <c r="H235" s="1">
+        <v>40197</v>
+      </c>
+      <c r="I235" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K235" s="1">
+        <v>40203</v>
+      </c>
+      <c r="L235" t="s">
+        <v>510</v>
+      </c>
+      <c r="O235" t="s">
+        <v>508</v>
+      </c>
+      <c r="P235" s="9"/>
+      <c r="Q235" s="9"/>
+      <c r="R235" s="9"/>
+      <c r="S235" s="9"/>
+    </row>
+    <row r="236" spans="1:19">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" t="s">
+        <v>13</v>
+      </c>
+      <c r="C236">
+        <v>57</v>
+      </c>
+      <c r="D236" t="s">
+        <v>28</v>
+      </c>
+      <c r="E236" t="s">
+        <v>37</v>
+      </c>
+      <c r="H236" s="1">
+        <v>40193</v>
+      </c>
+      <c r="I236" s="1">
+        <v>40199</v>
+      </c>
+      <c r="K236" s="1">
+        <v>40203</v>
+      </c>
+      <c r="L236" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="O236" t="s">
+        <v>508</v>
+      </c>
+      <c r="P236" s="9"/>
+      <c r="Q236" s="9"/>
+      <c r="R236" s="9"/>
+      <c r="S236" s="9"/>
+    </row>
+    <row r="237" spans="1:19">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>22</v>
+      </c>
+      <c r="C237">
+        <v>46</v>
+      </c>
+      <c r="D237" t="s">
+        <v>306</v>
+      </c>
+      <c r="E237" t="s">
+        <v>413</v>
+      </c>
+      <c r="H237" s="1">
+        <v>40195</v>
+      </c>
+      <c r="I237" s="1">
+        <v>40199</v>
+      </c>
+      <c r="K237" s="1">
+        <v>40203</v>
+      </c>
+      <c r="L237" t="s">
+        <v>512</v>
+      </c>
+      <c r="O237" t="s">
+        <v>508</v>
+      </c>
+      <c r="P237" s="9"/>
+      <c r="Q237" s="9"/>
+      <c r="R237" s="9"/>
+      <c r="S237" s="9"/>
+    </row>
+    <row r="238" spans="1:19">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>13</v>
+      </c>
+      <c r="C238">
+        <v>82</v>
+      </c>
+      <c r="D238" t="s">
+        <v>345</v>
+      </c>
+      <c r="E238" t="s">
+        <v>369</v>
+      </c>
+      <c r="H238" s="1">
+        <v>40188</v>
+      </c>
+      <c r="I238" s="1">
+        <v>40198</v>
+      </c>
+      <c r="K238" s="1">
+        <v>40203</v>
+      </c>
+      <c r="L238" t="s">
+        <v>513</v>
+      </c>
+      <c r="O238" t="s">
+        <v>508</v>
+      </c>
+      <c r="P238" s="9"/>
+      <c r="Q238" s="9"/>
+      <c r="R238" s="9"/>
+      <c r="S238" s="9"/>
+    </row>
+    <row r="239" spans="1:19">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>13</v>
+      </c>
+      <c r="C239">
+        <v>76</v>
+      </c>
+      <c r="D239" t="s">
+        <v>28</v>
+      </c>
+      <c r="E239" t="s">
+        <v>41</v>
+      </c>
+      <c r="H239" s="1">
+        <v>40195</v>
+      </c>
+      <c r="I239" s="1">
+        <v>40198</v>
+      </c>
+      <c r="K239" s="1">
+        <v>40204</v>
+      </c>
+      <c r="L239" t="s">
+        <v>514</v>
+      </c>
+      <c r="O239" t="s">
+        <v>508</v>
+      </c>
+      <c r="P239" s="9"/>
+      <c r="Q239" s="9"/>
+      <c r="R239" s="9"/>
+      <c r="S239" s="9"/>
+    </row>
+    <row r="240" spans="1:19">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>13</v>
+      </c>
+      <c r="C240">
+        <v>40</v>
+      </c>
+      <c r="D240" t="s">
+        <v>45</v>
+      </c>
+      <c r="E240" t="s">
+        <v>52</v>
+      </c>
+      <c r="H240" s="1">
+        <v>40196</v>
+      </c>
+      <c r="I240" s="1">
+        <v>40202</v>
+      </c>
+      <c r="K240" s="1">
+        <v>40204</v>
+      </c>
+      <c r="L240" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="O240" t="s">
+        <v>508</v>
+      </c>
+      <c r="P240" s="9"/>
+      <c r="Q240" s="9"/>
+      <c r="R240" s="9"/>
+      <c r="S240" s="9"/>
+    </row>
+    <row r="241" spans="1:19">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>13</v>
+      </c>
+      <c r="C241">
+        <v>65</v>
+      </c>
+      <c r="D241" t="s">
+        <v>45</v>
+      </c>
+      <c r="E241" t="s">
+        <v>55</v>
+      </c>
+      <c r="H241" s="1">
+        <v>40193</v>
+      </c>
+      <c r="I241" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K241" s="1">
+        <v>40204</v>
+      </c>
+      <c r="L241" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="O241" t="s">
+        <v>508</v>
+      </c>
+      <c r="P241" s="9"/>
+      <c r="Q241" s="9"/>
+      <c r="R241" s="9"/>
+      <c r="S241" s="9"/>
+    </row>
+    <row r="242" spans="1:19">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>22</v>
+      </c>
+      <c r="C242">
+        <v>74</v>
+      </c>
+      <c r="D242" t="s">
+        <v>28</v>
+      </c>
+      <c r="E242" t="s">
+        <v>37</v>
+      </c>
+      <c r="H242" s="1">
+        <v>40192</v>
+      </c>
+      <c r="I242" s="1">
+        <v>40201</v>
+      </c>
+      <c r="K242" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L242" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="O242" t="s">
+        <v>518</v>
+      </c>
+      <c r="P242" s="9"/>
+      <c r="Q242" s="9"/>
+      <c r="R242" s="9"/>
+      <c r="S242" s="9"/>
+    </row>
+    <row r="243" spans="1:19">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>22</v>
+      </c>
+      <c r="C243">
+        <v>58</v>
+      </c>
+      <c r="D243" t="s">
+        <v>215</v>
+      </c>
+      <c r="E243" t="s">
+        <v>519</v>
+      </c>
+      <c r="H243" s="1">
+        <v>40197</v>
+      </c>
+      <c r="I243" s="1">
+        <v>40202</v>
+      </c>
+      <c r="K243" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L243" t="s">
+        <v>520</v>
+      </c>
+      <c r="O243" t="s">
+        <v>518</v>
+      </c>
+      <c r="P243" s="9"/>
+      <c r="Q243" s="9"/>
+      <c r="R243" s="9"/>
+      <c r="S243" s="9"/>
+    </row>
+    <row r="244" spans="1:19">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>13</v>
+      </c>
+      <c r="C244">
+        <v>69</v>
+      </c>
+      <c r="D244" t="s">
+        <v>306</v>
+      </c>
+      <c r="E244" t="s">
+        <v>521</v>
+      </c>
+      <c r="H244" s="1">
+        <v>40194</v>
+      </c>
+      <c r="I244" s="1">
+        <v>40201</v>
+      </c>
+      <c r="K244" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L244" t="s">
+        <v>522</v>
+      </c>
+      <c r="O244" t="s">
+        <v>518</v>
+      </c>
+      <c r="P244" s="9"/>
+      <c r="Q244" s="9"/>
+      <c r="R244" s="9"/>
+      <c r="S244" s="9"/>
+    </row>
+    <row r="245" spans="1:19">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>22</v>
+      </c>
+      <c r="C245">
+        <v>72</v>
+      </c>
+      <c r="D245" t="s">
+        <v>306</v>
+      </c>
+      <c r="E245" t="s">
+        <v>523</v>
+      </c>
+      <c r="H245" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I245" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K245" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L245" t="s">
+        <v>524</v>
+      </c>
+      <c r="O245" t="s">
+        <v>518</v>
+      </c>
+      <c r="P245" s="9"/>
+      <c r="Q245" s="9"/>
+      <c r="R245" s="9"/>
+      <c r="S245" s="9"/>
+    </row>
+    <row r="246" spans="1:19">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>22</v>
+      </c>
+      <c r="C246">
+        <v>77</v>
+      </c>
+      <c r="D246" t="s">
+        <v>345</v>
+      </c>
+      <c r="E246" t="s">
+        <v>369</v>
+      </c>
+      <c r="H246" s="1">
+        <v>40194</v>
+      </c>
+      <c r="I246" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K246" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L246" t="s">
+        <v>525</v>
+      </c>
+      <c r="O246" t="s">
+        <v>518</v>
+      </c>
+      <c r="P246" s="9"/>
+      <c r="Q246" s="9"/>
+      <c r="R246" s="9"/>
+      <c r="S246" s="9"/>
+    </row>
+    <row r="247" spans="1:19">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>13</v>
+      </c>
+      <c r="C247">
+        <v>68</v>
+      </c>
+      <c r="D247" t="s">
+        <v>345</v>
+      </c>
+      <c r="E247" t="s">
+        <v>526</v>
+      </c>
+      <c r="H247" s="1">
+        <v>40195</v>
+      </c>
+      <c r="I247" s="1">
+        <v>40198</v>
+      </c>
+      <c r="J247" s="1">
+        <v>40202</v>
+      </c>
+      <c r="K247" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L247" t="s">
+        <v>527</v>
+      </c>
+      <c r="N247" t="s">
+        <v>428</v>
+      </c>
+      <c r="O247" t="s">
+        <v>518</v>
+      </c>
+      <c r="P247" s="9"/>
+      <c r="Q247" s="9"/>
+      <c r="R247" s="9"/>
+      <c r="S247" s="9"/>
+    </row>
+    <row r="248" spans="1:19">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>22</v>
+      </c>
+      <c r="C248">
+        <v>61</v>
+      </c>
+      <c r="D248" t="s">
+        <v>14</v>
+      </c>
+      <c r="E248" t="s">
+        <v>14</v>
+      </c>
+      <c r="H248" s="1">
+        <v>40183</v>
+      </c>
+      <c r="I248" s="1">
+        <v>40197</v>
+      </c>
+      <c r="K248" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L248" t="s">
+        <v>528</v>
+      </c>
+      <c r="O248" t="s">
+        <v>529</v>
+      </c>
+      <c r="P248" s="9"/>
+      <c r="Q248" s="9"/>
+      <c r="R248" s="9"/>
+      <c r="S248" s="9"/>
+    </row>
+    <row r="249" spans="1:19">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>22</v>
+      </c>
+      <c r="C249">
+        <v>66</v>
+      </c>
+      <c r="D249" t="s">
+        <v>45</v>
+      </c>
+      <c r="E249" t="s">
+        <v>394</v>
+      </c>
+      <c r="H249" s="1">
+        <v>40192</v>
+      </c>
+      <c r="I249" s="1">
+        <v>40194</v>
+      </c>
+      <c r="K249" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L249" t="s">
+        <v>530</v>
+      </c>
+      <c r="O249" t="s">
+        <v>529</v>
+      </c>
+      <c r="P249" s="9"/>
+      <c r="Q249" s="9"/>
+      <c r="R249" s="9"/>
+      <c r="S249" s="9"/>
+    </row>
+    <row r="250" spans="1:19">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>22</v>
+      </c>
+      <c r="C250">
+        <v>71</v>
+      </c>
+      <c r="D250" t="s">
+        <v>45</v>
+      </c>
+      <c r="E250" t="s">
+        <v>52</v>
+      </c>
+      <c r="H250" s="1">
+        <v>40189</v>
+      </c>
+      <c r="I250" s="1">
+        <v>40195</v>
+      </c>
+      <c r="K250" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L250" t="s">
+        <v>531</v>
+      </c>
+      <c r="O250" t="s">
+        <v>529</v>
+      </c>
+      <c r="P250" s="9"/>
+      <c r="Q250" s="9"/>
+      <c r="R250" s="9"/>
+      <c r="S250" s="9"/>
+    </row>
+    <row r="251" spans="1:19">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>13</v>
+      </c>
+      <c r="C251">
+        <v>71</v>
+      </c>
+      <c r="D251" t="s">
+        <v>45</v>
+      </c>
+      <c r="E251" t="s">
+        <v>164</v>
+      </c>
+      <c r="H251" s="1">
+        <v>40190</v>
+      </c>
+      <c r="I251" s="1">
+        <v>40198</v>
+      </c>
+      <c r="K251" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L251" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="O251" t="s">
+        <v>529</v>
+      </c>
+      <c r="P251" s="9"/>
+      <c r="Q251" s="9"/>
+      <c r="R251" s="9"/>
+      <c r="S251" s="9"/>
+    </row>
+    <row r="252" spans="1:19">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>13</v>
+      </c>
+      <c r="C252">
+        <v>59</v>
+      </c>
+      <c r="D252" t="s">
+        <v>45</v>
+      </c>
+      <c r="E252" t="s">
+        <v>408</v>
+      </c>
+      <c r="H252" s="1">
+        <v>40195</v>
+      </c>
+      <c r="I252" s="1">
+        <v>40199</v>
+      </c>
+      <c r="K252" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L252" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="O252" t="s">
+        <v>529</v>
+      </c>
+      <c r="P252" s="9"/>
+      <c r="Q252" s="9"/>
+      <c r="R252" s="9"/>
+      <c r="S252" s="9"/>
+    </row>
+    <row r="253" spans="1:19">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>22</v>
+      </c>
+      <c r="C253">
+        <v>63</v>
+      </c>
+      <c r="D253" t="s">
+        <v>45</v>
+      </c>
+      <c r="E253" t="s">
+        <v>55</v>
+      </c>
+      <c r="H253" s="1">
+        <v>40188</v>
+      </c>
+      <c r="I253" s="1">
+        <v>40195</v>
+      </c>
+      <c r="K253" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L253" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="O253" t="s">
+        <v>529</v>
+      </c>
+      <c r="P253" s="9"/>
+      <c r="Q253" s="9"/>
+      <c r="R253" s="9"/>
+      <c r="S253" s="9"/>
+    </row>
+    <row r="254" spans="1:19">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>22</v>
+      </c>
+      <c r="C254">
+        <v>34</v>
+      </c>
+      <c r="D254" t="s">
+        <v>345</v>
+      </c>
+      <c r="E254" t="s">
+        <v>369</v>
+      </c>
+      <c r="H254" s="1">
+        <v>40187</v>
+      </c>
+      <c r="I254" s="1">
+        <v>40198</v>
+      </c>
+      <c r="K254" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L254" t="s">
+        <v>535</v>
+      </c>
+      <c r="O254" t="s">
+        <v>529</v>
+      </c>
+      <c r="P254" s="9"/>
+      <c r="Q254" s="9"/>
+      <c r="R254" s="9"/>
+      <c r="S254" s="9"/>
+    </row>
+    <row r="255" spans="1:19">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>13</v>
+      </c>
+      <c r="C255">
+        <v>53</v>
+      </c>
+      <c r="D255" t="s">
+        <v>28</v>
+      </c>
+      <c r="E255" t="s">
+        <v>536</v>
+      </c>
+      <c r="H255" s="1">
+        <v>40199</v>
+      </c>
+      <c r="I255" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K255" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L255" t="s">
+        <v>537</v>
+      </c>
+      <c r="O255" t="s">
+        <v>529</v>
+      </c>
+      <c r="P255" s="9"/>
+      <c r="Q255" s="9"/>
+      <c r="R255" s="9"/>
+      <c r="S255" s="9"/>
+    </row>
+    <row r="256" spans="1:19">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>22</v>
+      </c>
+      <c r="C256">
+        <v>43</v>
+      </c>
+      <c r="D256" t="s">
+        <v>45</v>
+      </c>
+      <c r="E256" t="s">
+        <v>52</v>
+      </c>
+      <c r="H256" s="1">
+        <v>40200</v>
+      </c>
+      <c r="I256" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K256" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L256" t="s">
+        <v>538</v>
+      </c>
+      <c r="O256" t="s">
+        <v>529</v>
+      </c>
+      <c r="P256" s="9"/>
+      <c r="Q256" s="9"/>
+      <c r="R256" s="9"/>
+      <c r="S256" s="9"/>
+    </row>
+    <row r="257" spans="1:19">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" t="s">
+        <v>13</v>
+      </c>
+      <c r="C257">
+        <v>81</v>
+      </c>
+      <c r="D257" t="s">
+        <v>45</v>
+      </c>
+      <c r="E257" t="s">
+        <v>55</v>
+      </c>
+      <c r="H257" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I257" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K257" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L257" t="s">
+        <v>539</v>
+      </c>
+      <c r="O257" t="s">
+        <v>529</v>
+      </c>
+      <c r="P257" s="9"/>
+      <c r="Q257" s="9"/>
+      <c r="R257" s="9"/>
+      <c r="S257" s="9"/>
+    </row>
+    <row r="258" spans="1:19">
+      <c r="A258">
+        <v>257</v>
+      </c>
+      <c r="B258" t="s">
+        <v>22</v>
+      </c>
+      <c r="C258">
+        <v>63</v>
+      </c>
+      <c r="D258" t="s">
+        <v>45</v>
+      </c>
+      <c r="E258" t="s">
+        <v>55</v>
+      </c>
+      <c r="H258" s="1">
+        <v>40199</v>
+      </c>
+      <c r="I258" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K258" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L258" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="O258" t="s">
+        <v>529</v>
+      </c>
+      <c r="P258" s="9"/>
+      <c r="Q258" s="9"/>
+      <c r="R258" s="9"/>
+      <c r="S258" s="9"/>
+    </row>
+    <row r="259" spans="1:19">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>13</v>
+      </c>
+      <c r="C259">
+        <v>57</v>
+      </c>
+      <c r="D259" t="s">
+        <v>45</v>
+      </c>
+      <c r="E259" t="s">
+        <v>408</v>
+      </c>
+      <c r="H259" s="1">
+        <v>40192</v>
+      </c>
+      <c r="I259" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K259" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L259" t="s">
+        <v>541</v>
+      </c>
+      <c r="O259" t="s">
+        <v>529</v>
+      </c>
+      <c r="P259" s="9"/>
+      <c r="Q259" s="9"/>
+      <c r="R259" s="9"/>
+      <c r="S259" s="9"/>
+    </row>
+    <row r="260" spans="1:19">
+      <c r="A260">
+        <v>259</v>
+      </c>
+      <c r="B260" t="s">
+        <v>22</v>
+      </c>
+      <c r="C260">
+        <v>43</v>
+      </c>
+      <c r="D260" t="s">
+        <v>345</v>
+      </c>
+      <c r="E260" t="s">
+        <v>369</v>
+      </c>
+      <c r="H260" s="1">
+        <v>40194</v>
+      </c>
+      <c r="I260" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K260" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L260" t="s">
+        <v>542</v>
+      </c>
+      <c r="O260" t="s">
+        <v>529</v>
+      </c>
+      <c r="P260" s="9"/>
+      <c r="Q260" s="9"/>
+      <c r="R260" s="9"/>
+      <c r="S260" s="9"/>
+    </row>
+    <row r="261" spans="1:19">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>22</v>
+      </c>
+      <c r="C261">
+        <v>41</v>
+      </c>
+      <c r="D261" t="s">
+        <v>345</v>
+      </c>
+      <c r="E261" t="s">
+        <v>369</v>
+      </c>
+      <c r="H261" s="1">
+        <v>40197</v>
+      </c>
+      <c r="I261" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K261" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L261" t="s">
+        <v>543</v>
+      </c>
+      <c r="O261" t="s">
+        <v>529</v>
+      </c>
+      <c r="P261" s="9"/>
+      <c r="Q261" s="9"/>
+      <c r="R261" s="9"/>
+      <c r="S261" s="9"/>
+    </row>
+    <row r="262" spans="1:19">
+      <c r="A262">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>22</v>
+      </c>
+      <c r="C262">
+        <v>31</v>
+      </c>
+      <c r="D262" t="s">
+        <v>345</v>
+      </c>
+      <c r="E262" t="s">
+        <v>369</v>
+      </c>
+      <c r="H262" s="1">
+        <v>40193</v>
+      </c>
+      <c r="I262" s="1">
+        <v>40200</v>
+      </c>
+      <c r="K262" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L262" t="s">
+        <v>544</v>
+      </c>
+      <c r="O262" t="s">
+        <v>529</v>
+      </c>
+      <c r="P262" s="9"/>
+      <c r="Q262" s="9"/>
+      <c r="R262" s="9"/>
+      <c r="S262" s="9"/>
+    </row>
+    <row r="263" spans="1:19">
+      <c r="A263">
+        <v>262</v>
+      </c>
+      <c r="B263" t="s">
+        <v>13</v>
+      </c>
+      <c r="C263">
+        <v>37</v>
+      </c>
+      <c r="D263" t="s">
+        <v>45</v>
+      </c>
+      <c r="E263" t="s">
+        <v>164</v>
+      </c>
+      <c r="H263" s="1">
+        <v>40196</v>
+      </c>
+      <c r="I263" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K263" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L263" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="O263" t="s">
+        <v>546</v>
+      </c>
+      <c r="P263" s="9"/>
+      <c r="Q263" s="9"/>
+      <c r="R263" s="9"/>
+      <c r="S263" s="9"/>
+    </row>
+    <row r="264" spans="1:19">
+      <c r="A264">
+        <v>263</v>
+      </c>
+      <c r="B264" t="s">
+        <v>13</v>
+      </c>
+      <c r="C264">
+        <v>60</v>
+      </c>
+      <c r="D264" t="s">
+        <v>45</v>
+      </c>
+      <c r="E264" t="s">
+        <v>52</v>
+      </c>
+      <c r="H264" s="1">
+        <v>40200</v>
+      </c>
+      <c r="I264" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K264" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L264" t="s">
+        <v>547</v>
+      </c>
+      <c r="O264" t="s">
+        <v>546</v>
+      </c>
+      <c r="P264" s="9"/>
+      <c r="Q264" s="9"/>
+      <c r="R264" s="9"/>
+      <c r="S264" s="9"/>
+    </row>
+    <row r="265" spans="1:19">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265" t="s">
+        <v>13</v>
+      </c>
+      <c r="C265">
+        <v>63</v>
+      </c>
+      <c r="D265" t="s">
+        <v>45</v>
+      </c>
+      <c r="E265" t="s">
+        <v>52</v>
+      </c>
+      <c r="H265" s="1">
+        <v>40201</v>
+      </c>
+      <c r="I265" s="1">
+        <v>40204</v>
+      </c>
+      <c r="K265" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L265" t="s">
+        <v>548</v>
+      </c>
+      <c r="O265" t="s">
+        <v>546</v>
+      </c>
+      <c r="P265" s="9"/>
+      <c r="Q265" s="9"/>
+      <c r="R265" s="9"/>
+      <c r="S265" s="9"/>
+    </row>
+    <row r="266" spans="1:19">
+      <c r="A266">
+        <v>265</v>
+      </c>
+      <c r="B266" t="s">
+        <v>13</v>
+      </c>
+      <c r="C266">
+        <v>2</v>
+      </c>
+      <c r="D266" t="s">
+        <v>306</v>
+      </c>
+      <c r="E266" t="s">
+        <v>521</v>
+      </c>
+      <c r="H266" s="1">
+        <v>40203</v>
+      </c>
+      <c r="I266" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K266" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L266" t="s">
+        <v>549</v>
+      </c>
+      <c r="O266" t="s">
+        <v>546</v>
+      </c>
+      <c r="P266" s="9"/>
+      <c r="Q266" s="9"/>
+      <c r="R266" s="9"/>
+      <c r="S266" s="9"/>
+    </row>
+    <row r="267" spans="1:19">
+      <c r="A267">
+        <v>266</v>
+      </c>
+      <c r="B267" t="s">
+        <v>13</v>
+      </c>
+      <c r="C267">
+        <v>17</v>
+      </c>
+      <c r="D267" t="s">
+        <v>345</v>
+      </c>
+      <c r="E267" t="s">
+        <v>421</v>
+      </c>
+      <c r="H267" s="1">
+        <v>40199</v>
+      </c>
+      <c r="I267" s="1">
+        <v>40204</v>
+      </c>
+      <c r="K267" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L267" t="s">
+        <v>550</v>
+      </c>
+      <c r="O267" t="s">
+        <v>546</v>
+      </c>
+      <c r="P267" s="9"/>
+      <c r="Q267" s="9"/>
+      <c r="R267" s="9"/>
+      <c r="S267" s="9"/>
+    </row>
+    <row r="268" spans="1:19">
+      <c r="A268">
+        <v>267</v>
+      </c>
+      <c r="B268" t="s">
+        <v>13</v>
+      </c>
+      <c r="C268">
+        <v>75</v>
+      </c>
+      <c r="D268" t="s">
+        <v>345</v>
+      </c>
+      <c r="E268" t="s">
+        <v>369</v>
+      </c>
+      <c r="G268" t="s">
+        <v>370</v>
+      </c>
+      <c r="H268" s="1">
+        <v>40203</v>
+      </c>
+      <c r="I268" s="1">
+        <v>40205</v>
+      </c>
+      <c r="J268" s="1">
+        <v>40206</v>
+      </c>
+      <c r="K268" s="1">
+        <v>40206</v>
+      </c>
+      <c r="L268" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="N268" t="s">
+        <v>428</v>
+      </c>
+      <c r="O268" t="s">
+        <v>546</v>
+      </c>
+      <c r="P268" s="9"/>
+      <c r="Q268" s="9"/>
+      <c r="R268" s="9"/>
+      <c r="S268" s="9"/>
+    </row>
+    <row r="269" spans="1:19">
+      <c r="A269">
+        <v>268</v>
+      </c>
+      <c r="B269" t="s">
+        <v>13</v>
+      </c>
+      <c r="C269">
+        <v>75</v>
+      </c>
+      <c r="D269" t="s">
+        <v>45</v>
+      </c>
+      <c r="E269" t="s">
+        <v>408</v>
+      </c>
+      <c r="H269" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I269" s="1">
+        <v>40201</v>
+      </c>
+      <c r="K269" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L269" t="s">
+        <v>552</v>
+      </c>
+      <c r="O269" t="s">
+        <v>553</v>
+      </c>
+      <c r="P269" s="9"/>
+      <c r="Q269" s="9"/>
+      <c r="R269" s="9"/>
+      <c r="S269" s="9"/>
+    </row>
+    <row r="270" spans="1:19">
+      <c r="A270">
+        <v>269</v>
+      </c>
+      <c r="B270" t="s">
+        <v>13</v>
+      </c>
+      <c r="C270">
+        <v>76</v>
+      </c>
+      <c r="D270" t="s">
+        <v>45</v>
+      </c>
+      <c r="E270" t="s">
+        <v>408</v>
+      </c>
+      <c r="H270" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I270" s="1">
+        <v>40201</v>
+      </c>
+      <c r="K270" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L270" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="O270" t="s">
+        <v>553</v>
+      </c>
+      <c r="P270" s="9"/>
+      <c r="Q270" s="9"/>
+      <c r="R270" s="9"/>
+      <c r="S270" s="9"/>
+    </row>
+    <row r="271" spans="1:19">
+      <c r="A271">
+        <v>270</v>
+      </c>
+      <c r="B271" t="s">
+        <v>13</v>
+      </c>
+      <c r="C271">
+        <v>78</v>
+      </c>
+      <c r="D271" t="s">
+        <v>45</v>
+      </c>
+      <c r="E271" t="s">
+        <v>52</v>
+      </c>
+      <c r="H271" s="1">
+        <v>40202</v>
+      </c>
+      <c r="I271" s="1">
+        <v>40204</v>
+      </c>
+      <c r="K271" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L271" s="11" t="s">
+        <v>555</v>
+      </c>
+      <c r="O271" t="s">
+        <v>553</v>
+      </c>
+      <c r="P271" s="9"/>
+      <c r="Q271" s="9"/>
+      <c r="R271" s="9"/>
+      <c r="S271" s="9"/>
+    </row>
+    <row r="272" spans="1:19">
+      <c r="A272">
+        <v>271</v>
+      </c>
+      <c r="B272" t="s">
+        <v>13</v>
+      </c>
+      <c r="C272">
+        <v>64</v>
+      </c>
+      <c r="D272" t="s">
+        <v>45</v>
+      </c>
+      <c r="E272" t="s">
+        <v>408</v>
+      </c>
+      <c r="H272" s="1">
+        <v>40190</v>
+      </c>
+      <c r="I272" s="1">
+        <v>40193</v>
+      </c>
+      <c r="K272" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L272" t="s">
+        <v>556</v>
+      </c>
+      <c r="O272" t="s">
+        <v>553</v>
+      </c>
+      <c r="P272" s="9"/>
+      <c r="Q272" s="9"/>
+      <c r="R272" s="9"/>
+      <c r="S272" s="9"/>
+    </row>
+    <row r="273" spans="1:19">
+      <c r="A273">
+        <v>272</v>
+      </c>
+      <c r="B273" t="s">
+        <v>22</v>
+      </c>
+      <c r="C273">
+        <v>75</v>
+      </c>
+      <c r="D273" t="s">
+        <v>28</v>
+      </c>
+      <c r="E273" t="s">
+        <v>25</v>
+      </c>
+      <c r="H273" s="1">
+        <v>40195</v>
+      </c>
+      <c r="I273" s="1">
+        <v>40202</v>
+      </c>
+      <c r="K273" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L273" t="s">
+        <v>557</v>
+      </c>
+      <c r="O273" t="s">
+        <v>553</v>
+      </c>
+      <c r="P273" s="9"/>
+      <c r="Q273" s="9"/>
+      <c r="R273" s="9"/>
+      <c r="S273" s="9"/>
+    </row>
+    <row r="274" spans="1:19">
+      <c r="A274">
+        <v>273</v>
+      </c>
+      <c r="B274" t="s">
+        <v>22</v>
+      </c>
+      <c r="C274">
+        <v>67</v>
+      </c>
+      <c r="D274" t="s">
+        <v>345</v>
+      </c>
+      <c r="E274" t="s">
+        <v>526</v>
+      </c>
+      <c r="H274" s="1">
+        <v>40201</v>
+      </c>
+      <c r="I274" s="1">
+        <v>40202</v>
+      </c>
+      <c r="J274" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K274" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L274" t="s">
+        <v>558</v>
+      </c>
+      <c r="N274" t="s">
+        <v>428</v>
+      </c>
+      <c r="O274" t="s">
+        <v>553</v>
+      </c>
+      <c r="P274" s="9"/>
+      <c r="Q274" s="9"/>
+      <c r="R274" s="9"/>
+      <c r="S274" s="9"/>
+    </row>
+    <row r="275" spans="1:19">
+      <c r="A275">
+        <v>274</v>
+      </c>
+      <c r="B275" t="s">
+        <v>22</v>
+      </c>
+      <c r="C275">
+        <v>56</v>
+      </c>
+      <c r="D275" t="s">
+        <v>559</v>
+      </c>
+      <c r="E275" t="s">
+        <v>560</v>
+      </c>
+      <c r="H275" s="1">
+        <v>40197</v>
+      </c>
+      <c r="I275" s="1">
+        <v>40204</v>
+      </c>
+      <c r="K275" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L275" t="s">
+        <v>561</v>
+      </c>
+      <c r="O275" t="s">
+        <v>553</v>
+      </c>
+      <c r="P275" s="9"/>
+      <c r="Q275" s="9"/>
+      <c r="R275" s="9"/>
+      <c r="S275" s="9"/>
+    </row>
+    <row r="276" spans="1:19">
+      <c r="A276">
+        <v>275</v>
+      </c>
+      <c r="B276" t="s">
+        <v>13</v>
+      </c>
+      <c r="C276">
+        <v>80</v>
+      </c>
+      <c r="D276" t="s">
+        <v>45</v>
+      </c>
+      <c r="E276" t="s">
+        <v>52</v>
+      </c>
+      <c r="H276" s="1">
+        <v>40196</v>
+      </c>
+      <c r="I276" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K276" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L276" t="s">
+        <v>562</v>
+      </c>
+      <c r="O276" t="s">
+        <v>563</v>
+      </c>
+      <c r="P276" s="9"/>
+      <c r="Q276" s="9"/>
+      <c r="R276" s="9"/>
+      <c r="S276" s="9"/>
+    </row>
+    <row r="277" spans="1:19">
+      <c r="A277">
+        <v>276</v>
+      </c>
+      <c r="B277" t="s">
+        <v>13</v>
+      </c>
+      <c r="C277">
+        <v>54</v>
+      </c>
+      <c r="D277" t="s">
+        <v>45</v>
+      </c>
+      <c r="E277" t="s">
+        <v>52</v>
+      </c>
+      <c r="H277" s="1">
+        <v>40200</v>
+      </c>
+      <c r="I277" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K277" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L277" t="s">
+        <v>564</v>
+      </c>
+      <c r="O277" t="s">
+        <v>563</v>
+      </c>
+      <c r="P277" s="9"/>
+      <c r="Q277" s="9"/>
+      <c r="R277" s="9"/>
+      <c r="S277" s="9"/>
+    </row>
+    <row r="278" spans="1:19">
+      <c r="A278">
+        <v>277</v>
+      </c>
+      <c r="B278" t="s">
+        <v>13</v>
+      </c>
+      <c r="C278">
+        <v>6</v>
+      </c>
+      <c r="D278" t="s">
+        <v>345</v>
+      </c>
+      <c r="E278" t="s">
+        <v>369</v>
+      </c>
+      <c r="H278" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I278" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K278" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L278" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="O278" t="s">
+        <v>563</v>
+      </c>
+      <c r="P278" s="9"/>
+      <c r="Q278" s="9"/>
+      <c r="R278" s="9"/>
+      <c r="S278" s="9"/>
+    </row>
+    <row r="279" spans="1:19">
+      <c r="A279">
+        <v>278</v>
+      </c>
+      <c r="B279" t="s">
+        <v>13</v>
+      </c>
+      <c r="C279">
+        <v>5</v>
+      </c>
+      <c r="D279" t="s">
+        <v>345</v>
+      </c>
+      <c r="E279" t="s">
+        <v>566</v>
+      </c>
+      <c r="H279" s="1">
+        <v>40206</v>
+      </c>
+      <c r="I279" s="1">
+        <v>40206</v>
+      </c>
+      <c r="K279" s="1">
+        <v>40209</v>
+      </c>
+      <c r="L279" t="s">
+        <v>567</v>
+      </c>
+      <c r="O279" t="s">
+        <v>563</v>
+      </c>
+      <c r="P279" s="9"/>
+      <c r="Q279" s="9"/>
+      <c r="R279" s="9"/>
+      <c r="S279" s="9"/>
+    </row>
+    <row r="280" spans="1:19">
+      <c r="A280">
+        <v>279</v>
+      </c>
+      <c r="B280" t="s">
+        <v>13</v>
+      </c>
+      <c r="C280">
+        <v>28</v>
+      </c>
+      <c r="D280" t="s">
+        <v>345</v>
+      </c>
+      <c r="E280" t="s">
+        <v>566</v>
+      </c>
+      <c r="H280" s="1">
+        <v>40201</v>
+      </c>
+      <c r="I280" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K280" s="1">
+        <v>40208</v>
+      </c>
+      <c r="L280" t="s">
+        <v>568</v>
+      </c>
+      <c r="O280" t="s">
+        <v>563</v>
+      </c>
+      <c r="P280" s="9"/>
+      <c r="Q280" s="9"/>
+      <c r="R280" s="9"/>
+      <c r="S280" s="9"/>
+    </row>
+    <row r="281" spans="1:19">
+      <c r="A281">
+        <v>280</v>
+      </c>
+      <c r="B281" t="s">
+        <v>13</v>
+      </c>
+      <c r="C281">
+        <v>82</v>
+      </c>
+      <c r="D281" t="s">
+        <v>345</v>
+      </c>
+      <c r="E281" t="s">
+        <v>398</v>
+      </c>
+      <c r="H281" s="1">
+        <v>40199</v>
+      </c>
+      <c r="I281" s="1">
+        <v>40203</v>
+      </c>
+      <c r="K281" s="1">
+        <v>40208</v>
+      </c>
+      <c r="L281" t="s">
+        <v>569</v>
+      </c>
+      <c r="O281" t="s">
+        <v>563</v>
+      </c>
+      <c r="P281" s="9"/>
+      <c r="Q281" s="9"/>
+      <c r="R281" s="9"/>
+      <c r="S281" s="9"/>
+    </row>
+    <row r="282" spans="1:19">
+      <c r="A282">
+        <v>281</v>
+      </c>
+      <c r="B282" t="s">
+        <v>13</v>
+      </c>
+      <c r="C282">
+        <v>59</v>
+      </c>
+      <c r="D282" t="s">
+        <v>345</v>
+      </c>
+      <c r="E282" t="s">
+        <v>421</v>
+      </c>
+      <c r="H282" s="1">
+        <v>40199</v>
+      </c>
+      <c r="I282" s="1">
+        <v>40203</v>
+      </c>
+      <c r="J282" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K282" s="1">
+        <v>40208</v>
+      </c>
+      <c r="L282" t="s">
+        <v>570</v>
+      </c>
+      <c r="N282" t="s">
+        <v>428</v>
+      </c>
+      <c r="O282" t="s">
+        <v>563</v>
+      </c>
+      <c r="P282" s="9"/>
+      <c r="Q282" s="9"/>
+      <c r="R282" s="9"/>
+      <c r="S282" s="9"/>
+    </row>
+    <row r="283" spans="1:19">
+      <c r="A283">
+        <v>282</v>
+      </c>
+      <c r="B283" t="s">
+        <v>22</v>
+      </c>
+      <c r="C283">
+        <v>81</v>
+      </c>
+      <c r="D283" t="s">
+        <v>345</v>
+      </c>
+      <c r="E283" t="s">
+        <v>369</v>
+      </c>
+      <c r="H283" s="1">
+        <v>40202</v>
+      </c>
+      <c r="I283" s="1">
+        <v>40206</v>
+      </c>
+      <c r="K283" s="1">
+        <v>40208</v>
+      </c>
+      <c r="L283" t="s">
+        <v>571</v>
+      </c>
+      <c r="O283" t="s">
+        <v>563</v>
+      </c>
+      <c r="P283" s="9"/>
+      <c r="Q283" s="9"/>
+      <c r="R283" s="9"/>
+      <c r="S283" s="9"/>
+    </row>
+    <row r="284" spans="1:19">
+      <c r="A284">
+        <v>283</v>
+      </c>
+      <c r="B284" t="s">
+        <v>13</v>
+      </c>
+      <c r="C284">
+        <v>38</v>
+      </c>
+      <c r="D284" t="s">
+        <v>215</v>
+      </c>
+      <c r="E284" t="s">
+        <v>572</v>
+      </c>
+      <c r="H284" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="I284" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K284" s="1">
+        <v>40208</v>
+      </c>
+      <c r="L284" t="s">
+        <v>574</v>
+      </c>
+      <c r="O284" t="s">
+        <v>563</v>
+      </c>
+      <c r="P284" s="9"/>
+      <c r="Q284" s="9"/>
+      <c r="R284" s="9"/>
+      <c r="S284" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added 28 new cases from recent days
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="612">
   <si>
     <t>gender</t>
   </si>
@@ -1744,6 +1744,117 @@
   </si>
   <si>
     <t>A 38-year-old male from Yongzhou City, Hunan Province with onset of symptoms on 24 January 2014. He was admitted to hospital on 30 January and is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 44 year-old man from Taizhou City, Zhejiang Province, who became ill on 28 January and was admitted to hospital on 31 January. He is currently in a serious condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_04/en/index.html</t>
+  </si>
+  <si>
+    <t>A 8 year-old girl from Yongzhou City, Hunan Province, who became ill on 30 January and was admitted to hospital on 31 January. She is currently in a serious condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 35 year-old man from Xiamen City, Fujian Province, who became ill on 27 January and was admitted to hospital on 1 February. He is currently in serious condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>Zhongshan</t>
+  </si>
+  <si>
+    <t>A 37 year-old man from Zhongshan City, Guangdong Province, who became ill on 26 January and was admitted to hospital on 29 January and then transferred to the another hospital on 30 January. He is in a critical condition. He has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 63 year-old man from Shenzhen City, Guangdong Province, who became ill on 27 January and was admitted to hospital on 1 February and died on the same day. The patient had a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>Zhangzhou</t>
+  </si>
+  <si>
+    <t>A 27 year-old man from Zhangzhou City, Fujian Province, who became ill on 21 January and admitted to hospital on 31 January. He is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_05/en/index.html</t>
+  </si>
+  <si>
+    <t>Loudi</t>
+  </si>
+  <si>
+    <t>A 59 year-old man from Loudi City, Hunan Province, who became ill on 23 January and was admitted to hospital on 31 January. He died on 3 February. The patient had a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>A 2 year-old female from Zhongshan City, Guangdong Province, who became ill on 31 January and was admitted to hospital on the same day. She is currently in a mild condition. The patient has a history of exposure to live poultry and a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 76 year old woman from Huizhou City, Guangdong Province, who became ill on 27 January and was admitted to hospital on 1 February. She is currently in a serious condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 42 year-old man from Hangzhou City, Zhejiang Province, who became ill on 25 January and was admitted to hospital on 30 January. He is currently in a severe condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_05bis/en/index.html</t>
+  </si>
+  <si>
+    <t>An 84 year-old man from Hangzhou City, Zhejiang Province, who became ill on 24 January and was admitted to hospital on 28 January. He is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>Jinhua</t>
+  </si>
+  <si>
+    <t>A 56 year-old man from Jinhua City, Zhejiang Province, who became ill on 24 January and was admitted to hospital on 1 February. He is currently in a severe condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 51 year-old man from Shaoxing City, Zhejiang Province, who became ill on 27 January and was admitted on 1 February. He is currently in a critical condition. The patient has history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 4 year-old girl from Zhaoqing City, Guangdong Province, who became ill on 26 January and was admitted to hospital on 3 February. She is currently in a mild condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 76 year-old man from Yangjiang City, Guangdong Province, who became ill on 27 January and was admitted to hospital on 1 February. He died on 3 February. The patient had a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 52 year-old man from Huizhou City, Guangdong Province, who became ill on 25 January and was admitted to hospital on 2 February. He died on 3 February. The patient had a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 59 year-old woman from Wuxi City, Jiangsu Province, who became ill on 26 January and was admitted to hospital on 29 January. She is currently in a critical condition. The patient has history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 67 year-old farmer from Shaoxing City, Zhejiang Province, who became ill on 28 January and admitted to hospital on 2 February and transferred to another hospital on 4 February. He is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_07/en/index.html</t>
+  </si>
+  <si>
+    <t>A 35 year-old woman from Wenzhou City, Zhejiang Province, who became ill on 23 January and was admitted to hospital on 30 January and transferred to another hospital on 3 February. She is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 59 year-old woman from Hangzhou City, Zhejiang Province, who became ill on 21 January and admitted to hospital on 30 January and transferred to another hospital on 4 February. She is currently in a severe condition. The patient has a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>A 49 year-old farmer from Hangzhou City, Zhejiang Province, who became ill on 21 January and was admitted to hospital on 28 January and transferred to another hospital on 4 February. He is currently in a critical condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 36 year-old man from Quanzhou City, Fujian Province, who became ill on 30 January and was admitted to hospital on 2 February and transferred to another hospital on 4 February. He is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 5 year-old girl from Zhaoqing City, Guangdong Province, who became ill on 30 January and was admitted to hospital on the same day. She currently has a mild illness. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 42 year-old man from Zhaoqing City, Guangdong Province, who became ill on 27 January and was admitted to hospital on 28 January and transferred to another hospital on 4 February. He is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 49 year-old man from Foshan City, Guangdong Province, who became ill on 26 January and was admitted to hospital on 30 January and transferred to another hospital on 2 February. He is currently in a severe condition.</t>
+  </si>
+  <si>
+    <t>A 56 year-old man from Shenzhen City, Guangdong Province, who became ill on 29 January and was admitted to hospital on 2 February and transferred to another hospital on 3 February. He is currently in a critical condition. The patient has a history of exposure to live poultry market.</t>
+  </si>
+  <si>
+    <t>Nanning</t>
+  </si>
+  <si>
+    <t>Heng County</t>
+  </si>
+  <si>
+    <t>A 41 year-old woman from Heng County of Nanning City, Guangxi Province, who became ill on 27 January. She was working in Zhongshan City, Guangdong Province and returned to Heng County on 28 January. She was admitted to hospital on 3 February and is currently in a critical condition.</t>
   </si>
 </sst>
 </file>
@@ -1842,8 +1953,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="365">
+  <cellStyleXfs count="375">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2225,7 +2346,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="365">
+  <cellStyles count="375">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2408,6 +2529,11 @@
     <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2590,6 +2716,11 @@
     <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -2611,8 +2742,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S284" totalsRowShown="0">
-  <autoFilter ref="A1:S284"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S311" totalsRowShown="0">
+  <autoFilter ref="A1:S311"/>
   <tableColumns count="19">
     <tableColumn id="1" name="number"/>
     <tableColumn id="2" name="gender"/>
@@ -2960,13 +3091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S284"/>
+  <dimension ref="A1:S311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F253" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F280" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="E272" sqref="E272"/>
+      <selection pane="bottomRight" activeCell="F297" sqref="F297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12990,6 +13121,905 @@
       <c r="R284" s="9"/>
       <c r="S284" s="9"/>
     </row>
+    <row r="285" spans="1:19">
+      <c r="A285">
+        <v>284</v>
+      </c>
+      <c r="B285" t="s">
+        <v>13</v>
+      </c>
+      <c r="C285">
+        <v>44</v>
+      </c>
+      <c r="D285" t="s">
+        <v>45</v>
+      </c>
+      <c r="E285" t="s">
+        <v>476</v>
+      </c>
+      <c r="H285" s="1">
+        <v>40205</v>
+      </c>
+      <c r="I285" s="1">
+        <v>40208</v>
+      </c>
+      <c r="K285" s="1">
+        <v>40210</v>
+      </c>
+      <c r="L285" t="s">
+        <v>575</v>
+      </c>
+      <c r="O285" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="286" spans="1:19">
+      <c r="A286">
+        <v>285</v>
+      </c>
+      <c r="B286" t="s">
+        <v>22</v>
+      </c>
+      <c r="C286">
+        <v>8</v>
+      </c>
+      <c r="D286" t="s">
+        <v>215</v>
+      </c>
+      <c r="E286" t="s">
+        <v>572</v>
+      </c>
+      <c r="H286" s="1">
+        <v>40207</v>
+      </c>
+      <c r="I286" s="1">
+        <v>40208</v>
+      </c>
+      <c r="K286" s="1">
+        <v>40210</v>
+      </c>
+      <c r="L286" t="s">
+        <v>577</v>
+      </c>
+      <c r="O286" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="287" spans="1:19">
+      <c r="A287">
+        <v>286</v>
+      </c>
+      <c r="B287" t="s">
+        <v>13</v>
+      </c>
+      <c r="C287">
+        <v>35</v>
+      </c>
+      <c r="D287" t="s">
+        <v>306</v>
+      </c>
+      <c r="E287" t="s">
+        <v>521</v>
+      </c>
+      <c r="H287" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I287" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K287" s="1">
+        <v>40210</v>
+      </c>
+      <c r="L287" t="s">
+        <v>578</v>
+      </c>
+      <c r="O287" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="288" spans="1:19">
+      <c r="A288">
+        <v>287</v>
+      </c>
+      <c r="B288" t="s">
+        <v>13</v>
+      </c>
+      <c r="C288">
+        <v>37</v>
+      </c>
+      <c r="D288" t="s">
+        <v>345</v>
+      </c>
+      <c r="E288" t="s">
+        <v>579</v>
+      </c>
+      <c r="H288" s="1">
+        <v>40203</v>
+      </c>
+      <c r="I288" s="1">
+        <v>40206</v>
+      </c>
+      <c r="K288" s="1">
+        <v>40210</v>
+      </c>
+      <c r="L288" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="O288" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="289" spans="1:15">
+      <c r="A289">
+        <v>288</v>
+      </c>
+      <c r="B289" t="s">
+        <v>13</v>
+      </c>
+      <c r="C289">
+        <v>63</v>
+      </c>
+      <c r="D289" t="s">
+        <v>345</v>
+      </c>
+      <c r="E289" t="s">
+        <v>369</v>
+      </c>
+      <c r="H289" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I289" s="1">
+        <v>40209</v>
+      </c>
+      <c r="J289" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K289" s="1">
+        <v>40210</v>
+      </c>
+      <c r="L289" t="s">
+        <v>581</v>
+      </c>
+      <c r="N289" t="s">
+        <v>428</v>
+      </c>
+      <c r="O289" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="290" spans="1:15">
+      <c r="A290">
+        <v>289</v>
+      </c>
+      <c r="B290" t="s">
+        <v>13</v>
+      </c>
+      <c r="C290">
+        <v>27</v>
+      </c>
+      <c r="D290" t="s">
+        <v>306</v>
+      </c>
+      <c r="E290" t="s">
+        <v>582</v>
+      </c>
+      <c r="H290" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I290" s="1">
+        <v>40208</v>
+      </c>
+      <c r="K290" s="1">
+        <v>40211</v>
+      </c>
+      <c r="L290" t="s">
+        <v>583</v>
+      </c>
+      <c r="O290" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="291" spans="1:15">
+      <c r="A291">
+        <v>290</v>
+      </c>
+      <c r="B291" t="s">
+        <v>13</v>
+      </c>
+      <c r="C291">
+        <v>59</v>
+      </c>
+      <c r="D291" t="s">
+        <v>215</v>
+      </c>
+      <c r="E291" t="s">
+        <v>585</v>
+      </c>
+      <c r="H291" s="1">
+        <v>40200</v>
+      </c>
+      <c r="I291" s="1">
+        <v>40208</v>
+      </c>
+      <c r="J291" s="1">
+        <v>40211</v>
+      </c>
+      <c r="K291" s="1">
+        <v>40211</v>
+      </c>
+      <c r="L291" t="s">
+        <v>586</v>
+      </c>
+      <c r="N291" t="s">
+        <v>428</v>
+      </c>
+      <c r="O291" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="292" spans="1:15">
+      <c r="A292">
+        <v>291</v>
+      </c>
+      <c r="B292" t="s">
+        <v>22</v>
+      </c>
+      <c r="C292">
+        <v>2</v>
+      </c>
+      <c r="D292" t="s">
+        <v>345</v>
+      </c>
+      <c r="E292" t="s">
+        <v>579</v>
+      </c>
+      <c r="H292" s="1">
+        <v>40208</v>
+      </c>
+      <c r="I292" s="1">
+        <v>40208</v>
+      </c>
+      <c r="K292" s="1">
+        <v>40211</v>
+      </c>
+      <c r="L292" t="s">
+        <v>587</v>
+      </c>
+      <c r="O292" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="293" spans="1:15">
+      <c r="A293">
+        <v>292</v>
+      </c>
+      <c r="B293" t="s">
+        <v>22</v>
+      </c>
+      <c r="C293">
+        <v>76</v>
+      </c>
+      <c r="D293" t="s">
+        <v>345</v>
+      </c>
+      <c r="E293" t="s">
+        <v>105</v>
+      </c>
+      <c r="H293" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I293" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K293" s="1">
+        <v>40211</v>
+      </c>
+      <c r="L293" t="s">
+        <v>588</v>
+      </c>
+      <c r="O293" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="294" spans="1:15">
+      <c r="A294">
+        <v>293</v>
+      </c>
+      <c r="B294" t="s">
+        <v>13</v>
+      </c>
+      <c r="C294">
+        <v>42</v>
+      </c>
+      <c r="D294" t="s">
+        <v>45</v>
+      </c>
+      <c r="E294" t="s">
+        <v>52</v>
+      </c>
+      <c r="H294" s="1">
+        <v>40202</v>
+      </c>
+      <c r="I294" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K294" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L294" t="s">
+        <v>589</v>
+      </c>
+      <c r="O294" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="295" spans="1:15">
+      <c r="A295">
+        <v>294</v>
+      </c>
+      <c r="B295" t="s">
+        <v>13</v>
+      </c>
+      <c r="C295">
+        <v>84</v>
+      </c>
+      <c r="D295" t="s">
+        <v>45</v>
+      </c>
+      <c r="E295" t="s">
+        <v>52</v>
+      </c>
+      <c r="H295" s="1">
+        <v>40201</v>
+      </c>
+      <c r="I295" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K295" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L295" t="s">
+        <v>591</v>
+      </c>
+      <c r="O295" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="296" spans="1:15">
+      <c r="A296">
+        <v>295</v>
+      </c>
+      <c r="B296" t="s">
+        <v>13</v>
+      </c>
+      <c r="C296">
+        <v>56</v>
+      </c>
+      <c r="D296" t="s">
+        <v>45</v>
+      </c>
+      <c r="E296" t="s">
+        <v>592</v>
+      </c>
+      <c r="H296" s="1">
+        <v>40201</v>
+      </c>
+      <c r="I296" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K296" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L296" t="s">
+        <v>593</v>
+      </c>
+      <c r="O296" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="297" spans="1:15">
+      <c r="A297">
+        <v>296</v>
+      </c>
+      <c r="B297" t="s">
+        <v>13</v>
+      </c>
+      <c r="C297">
+        <v>51</v>
+      </c>
+      <c r="D297" t="s">
+        <v>45</v>
+      </c>
+      <c r="E297" t="s">
+        <v>394</v>
+      </c>
+      <c r="H297" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I297" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K297" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L297" t="s">
+        <v>594</v>
+      </c>
+      <c r="O297" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="298" spans="1:15">
+      <c r="A298">
+        <v>297</v>
+      </c>
+      <c r="B298" t="s">
+        <v>22</v>
+      </c>
+      <c r="C298">
+        <v>4</v>
+      </c>
+      <c r="D298" t="s">
+        <v>345</v>
+      </c>
+      <c r="E298" t="s">
+        <v>566</v>
+      </c>
+      <c r="H298" s="1">
+        <v>40203</v>
+      </c>
+      <c r="I298" s="1">
+        <v>40211</v>
+      </c>
+      <c r="K298" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L298" t="s">
+        <v>595</v>
+      </c>
+      <c r="O298" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="299" spans="1:15">
+      <c r="A299">
+        <v>298</v>
+      </c>
+      <c r="B299" t="s">
+        <v>13</v>
+      </c>
+      <c r="C299">
+        <v>76</v>
+      </c>
+      <c r="D299" t="s">
+        <v>345</v>
+      </c>
+      <c r="E299" t="s">
+        <v>378</v>
+      </c>
+      <c r="H299" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I299" s="1">
+        <v>40209</v>
+      </c>
+      <c r="J299" s="1">
+        <v>40211</v>
+      </c>
+      <c r="K299" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L299" t="s">
+        <v>596</v>
+      </c>
+      <c r="N299" t="s">
+        <v>428</v>
+      </c>
+      <c r="O299" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="300" spans="1:15">
+      <c r="A300">
+        <v>299</v>
+      </c>
+      <c r="B300" t="s">
+        <v>13</v>
+      </c>
+      <c r="C300">
+        <v>52</v>
+      </c>
+      <c r="D300" t="s">
+        <v>345</v>
+      </c>
+      <c r="E300" t="s">
+        <v>105</v>
+      </c>
+      <c r="H300" s="1">
+        <v>40202</v>
+      </c>
+      <c r="I300" s="1">
+        <v>40210</v>
+      </c>
+      <c r="J300" s="1">
+        <v>40211</v>
+      </c>
+      <c r="K300" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L300" t="s">
+        <v>597</v>
+      </c>
+      <c r="N300" t="s">
+        <v>428</v>
+      </c>
+      <c r="O300" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="301" spans="1:15">
+      <c r="A301">
+        <v>300</v>
+      </c>
+      <c r="B301" t="s">
+        <v>22</v>
+      </c>
+      <c r="C301">
+        <v>59</v>
+      </c>
+      <c r="D301" t="s">
+        <v>28</v>
+      </c>
+      <c r="E301" t="s">
+        <v>41</v>
+      </c>
+      <c r="H301" s="1">
+        <v>40203</v>
+      </c>
+      <c r="I301" s="1">
+        <v>40206</v>
+      </c>
+      <c r="K301" s="1">
+        <v>40212</v>
+      </c>
+      <c r="L301" t="s">
+        <v>598</v>
+      </c>
+      <c r="O301" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="302" spans="1:15">
+      <c r="A302">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>13</v>
+      </c>
+      <c r="C302">
+        <v>67</v>
+      </c>
+      <c r="D302" t="s">
+        <v>45</v>
+      </c>
+      <c r="E302" t="s">
+        <v>394</v>
+      </c>
+      <c r="H302" s="1">
+        <v>40205</v>
+      </c>
+      <c r="I302" s="1">
+        <v>40210</v>
+      </c>
+      <c r="K302" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L302" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="O302" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="303" spans="1:15">
+      <c r="A303">
+        <v>302</v>
+      </c>
+      <c r="B303" t="s">
+        <v>22</v>
+      </c>
+      <c r="C303">
+        <v>35</v>
+      </c>
+      <c r="D303" t="s">
+        <v>45</v>
+      </c>
+      <c r="E303" t="s">
+        <v>164</v>
+      </c>
+      <c r="H303" s="1">
+        <v>40200</v>
+      </c>
+      <c r="I303" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K303" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L303" s="11" t="s">
+        <v>601</v>
+      </c>
+      <c r="O303" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="304" spans="1:15">
+      <c r="A304">
+        <v>303</v>
+      </c>
+      <c r="B304" t="s">
+        <v>22</v>
+      </c>
+      <c r="C304">
+        <v>59</v>
+      </c>
+      <c r="D304" t="s">
+        <v>45</v>
+      </c>
+      <c r="E304" t="s">
+        <v>52</v>
+      </c>
+      <c r="H304" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I304" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K304" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L304" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="O304" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="305" spans="1:19">
+      <c r="A305">
+        <v>304</v>
+      </c>
+      <c r="B305" t="s">
+        <v>13</v>
+      </c>
+      <c r="C305">
+        <v>49</v>
+      </c>
+      <c r="D305" t="s">
+        <v>45</v>
+      </c>
+      <c r="E305" t="s">
+        <v>52</v>
+      </c>
+      <c r="H305" s="1">
+        <v>40198</v>
+      </c>
+      <c r="I305" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K305" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L305" s="11" t="s">
+        <v>603</v>
+      </c>
+      <c r="O305" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="306" spans="1:19">
+      <c r="A306">
+        <v>305</v>
+      </c>
+      <c r="B306" t="s">
+        <v>13</v>
+      </c>
+      <c r="C306">
+        <v>36</v>
+      </c>
+      <c r="D306" t="s">
+        <v>306</v>
+      </c>
+      <c r="E306" t="s">
+        <v>413</v>
+      </c>
+      <c r="H306" s="1">
+        <v>40207</v>
+      </c>
+      <c r="I306" s="1">
+        <v>40210</v>
+      </c>
+      <c r="K306" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L306" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="O306" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="307" spans="1:19">
+      <c r="A307">
+        <v>306</v>
+      </c>
+      <c r="B307" t="s">
+        <v>22</v>
+      </c>
+      <c r="C307">
+        <v>5</v>
+      </c>
+      <c r="D307" t="s">
+        <v>345</v>
+      </c>
+      <c r="E307" t="s">
+        <v>566</v>
+      </c>
+      <c r="H307" s="1">
+        <v>40207</v>
+      </c>
+      <c r="I307" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K307" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L307" t="s">
+        <v>605</v>
+      </c>
+      <c r="O307" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="308" spans="1:19">
+      <c r="A308">
+        <v>307</v>
+      </c>
+      <c r="B308" t="s">
+        <v>13</v>
+      </c>
+      <c r="C308">
+        <v>42</v>
+      </c>
+      <c r="D308" t="s">
+        <v>345</v>
+      </c>
+      <c r="E308" t="s">
+        <v>566</v>
+      </c>
+      <c r="H308" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I308" s="1">
+        <v>40205</v>
+      </c>
+      <c r="K308" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L308" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="O308" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="309" spans="1:19">
+      <c r="A309">
+        <v>308</v>
+      </c>
+      <c r="B309" t="s">
+        <v>13</v>
+      </c>
+      <c r="C309">
+        <v>49</v>
+      </c>
+      <c r="D309" t="s">
+        <v>345</v>
+      </c>
+      <c r="E309" t="s">
+        <v>398</v>
+      </c>
+      <c r="H309" s="1">
+        <v>40203</v>
+      </c>
+      <c r="I309" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K309" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L309" t="s">
+        <v>607</v>
+      </c>
+      <c r="O309" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="310" spans="1:19">
+      <c r="A310">
+        <v>309</v>
+      </c>
+      <c r="B310" t="s">
+        <v>13</v>
+      </c>
+      <c r="C310">
+        <v>56</v>
+      </c>
+      <c r="D310" t="s">
+        <v>345</v>
+      </c>
+      <c r="E310" t="s">
+        <v>369</v>
+      </c>
+      <c r="H310" s="1">
+        <v>40206</v>
+      </c>
+      <c r="I310" s="1">
+        <v>40210</v>
+      </c>
+      <c r="K310" s="1">
+        <v>40213</v>
+      </c>
+      <c r="L310" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="O310" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="311" spans="1:19">
+      <c r="A311">
+        <v>310</v>
+      </c>
+      <c r="B311" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C311" s="9">
+        <v>41</v>
+      </c>
+      <c r="D311" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="E311" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="F311" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="G311" s="9"/>
+      <c r="H311" s="10">
+        <v>40204</v>
+      </c>
+      <c r="I311" s="10">
+        <v>40211</v>
+      </c>
+      <c r="J311" s="10"/>
+      <c r="K311" s="10">
+        <v>40213</v>
+      </c>
+      <c r="L311" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="M311" s="9"/>
+      <c r="N311" s="9"/>
+      <c r="O311" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="P311" s="9"/>
+      <c r="Q311" s="9"/>
+      <c r="R311" s="9"/>
+      <c r="S311" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added 29 more recent #H7N9 cases to the Epidemic site: http://epidemic.bio.ed.ac.uk/influenza_H7N9_background
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="41540" windowHeight="17320" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="25360" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="647">
   <si>
     <t>gender</t>
   </si>
@@ -1882,6 +1882,84 @@
   </si>
   <si>
     <t>A 73 year-old man from Northern Beijing who became ill on 30 January and was admitted to hospital on 2 February and was transferred to another hospital on 5 February 2014. He is in critical condition . The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 54 year-old man from Hangzhou City, Zhejiang Province, who became ill on 1 February and was admitted to hospital on 4 February. He is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 76 year-old woman from Taizhou City, Zhejiang Province, who became ill on 24 January and was admitted to hospital on 31 January. She is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 81 year-old man from Fuzhou City, Fujian Province, who became ill on 30 January and was admitted to hospital on 2 February and discharged from hospital on 6 February at the request of his family and died at home on the same day. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 21 year-old woman from Loudi City, Hunan Province, who became ill on 30 January and was admitted to hospital on 1 February and then transferred to another hospital on 2 February. She is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 48 year-old man from Zhaoqing City, Guangdong Province, who became ill on 28 January. He was admitted to hospital on 30 January and then transferred to a hospital in Guangzhou City on 5 February 2014. He is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 62 year-old man from Zhaoqing City, Guangdong Province, who became ill on 1 February and was admitted to hospital on 2 February. He is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 59 year-old woman from Guangzhou City, Guangdong Province, who became ill on 27 January ad was admitted to hospital on 1 February. She is currently in a critical condition. The patient has history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 53 year-old man from Taizhou City, Jiangsu Province, who became ill on 1 February and was admitted to hospital on 8 February. He is currently in a severe condition.</t>
+  </si>
+  <si>
+    <t>A 61 year-old man from Hangzhou City, Zhejiang Province, who became ill on 29 January and was admitted to hospital on 2 February. He is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 38 year-old man from Shaoyang City, Hunan Province , who became ill on 27 January and was admitted to hospital on 2 February. He is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 81 year-old woman from Shenzhen City, Guangdong Province, who became ill on 31 January and was admitted to a hospital on 7 February. She died on the same day. The patient had a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 11 year-old boy from Zhaoqing City, Guangdong Province, who became ill on 5 February and went to hospital on the same day. He is currently in a stable condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 68 year-old farmer from Shaoxing City, Zhejiang Province, who became ill on 5 February and was admitted to hospital on 7 February. He is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>Anqing</t>
+  </si>
+  <si>
+    <t>A 66 year-old man from Anqing Prefecture, Anhui Province, who became ill on 1 February and was admitted to hospital on 7 February. He is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 67 year-old farmer from Jiaxing City, Zhejiang Province, who became ill on 3 February and was admitted to hospital on 8 February. He is currently in a critical condition</t>
+  </si>
+  <si>
+    <t>A 47 year-old woman from Wenzhou City, Zhejiang Province, who became ill on 3 February and was admitted to hospital on 7 February. She is currently in a severe condition. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 62 year-old farmer from Lishui City, Zhejiang Province, who became ill on 29 January and was admitted to hospital on 6 February. He is currently in a critical condition. The patient has a history of exposure to a live poultry.</t>
+  </si>
+  <si>
+    <t>Fuyang</t>
+  </si>
+  <si>
+    <t>A 56 year-old farmer from Fuyang City, Anhui Province, who became ill on 3 February and was admitted to hospital on 7 February. He died the same evening. The patient had a history or exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 5 year-old girl from Guangzhou City, Guangdong Province, who became ill on 1 February and was admitted to hospital on 3 February. She recovered and was discharged from hospital on 7 February. The patient has a history of exposure to a live poultry market.</t>
+  </si>
+  <si>
+    <t>A 70 year-old farmer from Hangzhou City, Zhejiang Province, who became ill on 4 February and was admitted to hospital on 5 February and transferred to another hospital on 9 February. He is currently in a critical condition. The patient has history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 23 year-old man from Loudi City, Hunan Province, who became ill on 8 February and was admitted to hospital on 9 February. He is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 65-year old man from Hong Kong SAR who became ill on 8 February and was admitted to a hospital on 11 February. He has underlying medical conditions and is currently in a critical condition. The patient travelled to Kaiping, Guangdong Province, in China from 24 January to 9 February and stayed with his family. Contact tracing is under way and investigations are ongoing.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_11/en/index.html</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_02_14/en/index.html</t>
   </si>
 </sst>
 </file>
@@ -1980,8 +2058,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="415">
+  <cellStyleXfs count="419">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2413,7 +2495,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="415">
+  <cellStyles count="419">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2621,6 +2703,8 @@
     <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2828,6 +2912,8 @@
     <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -2849,8 +2935,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S319" totalsRowShown="0">
-  <autoFilter ref="A1:S319"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S341" totalsRowShown="0">
+  <autoFilter ref="A1:S341"/>
   <tableColumns count="19">
     <tableColumn id="1" name="number"/>
     <tableColumn id="2" name="gender"/>
@@ -3198,13 +3284,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S319"/>
+  <dimension ref="A1:S341"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F288" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F310" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="D324" sqref="D324"/>
+      <selection pane="bottomRight" activeCell="L318" sqref="L318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14392,6 +14478,728 @@
         <v>612</v>
       </c>
     </row>
+    <row r="320" spans="1:19">
+      <c r="A320">
+        <v>319</v>
+      </c>
+      <c r="B320" t="s">
+        <v>13</v>
+      </c>
+      <c r="C320">
+        <v>54</v>
+      </c>
+      <c r="D320" t="s">
+        <v>45</v>
+      </c>
+      <c r="E320" t="s">
+        <v>52</v>
+      </c>
+      <c r="H320" s="1">
+        <v>40209</v>
+      </c>
+      <c r="I320" s="1">
+        <v>40212</v>
+      </c>
+      <c r="K320" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L320" t="s">
+        <v>621</v>
+      </c>
+      <c r="O320" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="321" spans="1:15">
+      <c r="A321">
+        <v>320</v>
+      </c>
+      <c r="B321" t="s">
+        <v>22</v>
+      </c>
+      <c r="C321">
+        <v>76</v>
+      </c>
+      <c r="D321" t="s">
+        <v>45</v>
+      </c>
+      <c r="E321" t="s">
+        <v>476</v>
+      </c>
+      <c r="H321" s="1">
+        <v>40201</v>
+      </c>
+      <c r="I321" s="1">
+        <v>40208</v>
+      </c>
+      <c r="K321" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L321" t="s">
+        <v>622</v>
+      </c>
+      <c r="O321" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="322" spans="1:15">
+      <c r="A322">
+        <v>321</v>
+      </c>
+      <c r="B322" t="s">
+        <v>13</v>
+      </c>
+      <c r="C322">
+        <v>81</v>
+      </c>
+      <c r="D322" t="s">
+        <v>306</v>
+      </c>
+      <c r="E322" t="s">
+        <v>392</v>
+      </c>
+      <c r="H322" s="1">
+        <v>40207</v>
+      </c>
+      <c r="I322" s="1">
+        <v>40210</v>
+      </c>
+      <c r="J322" s="1">
+        <v>40214</v>
+      </c>
+      <c r="K322" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L322" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="N322" t="s">
+        <v>428</v>
+      </c>
+      <c r="O322" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="323" spans="1:15">
+      <c r="A323">
+        <v>322</v>
+      </c>
+      <c r="B323" t="s">
+        <v>22</v>
+      </c>
+      <c r="C323">
+        <v>21</v>
+      </c>
+      <c r="D323" t="s">
+        <v>215</v>
+      </c>
+      <c r="E323" t="s">
+        <v>585</v>
+      </c>
+      <c r="H323" s="1">
+        <v>40207</v>
+      </c>
+      <c r="I323" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K323" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L323" s="11" t="s">
+        <v>624</v>
+      </c>
+      <c r="O323" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="324" spans="1:15">
+      <c r="A324">
+        <v>323</v>
+      </c>
+      <c r="B324" t="s">
+        <v>13</v>
+      </c>
+      <c r="C324">
+        <v>48</v>
+      </c>
+      <c r="D324" t="s">
+        <v>566</v>
+      </c>
+      <c r="E324" t="s">
+        <v>345</v>
+      </c>
+      <c r="H324" s="1">
+        <v>40205</v>
+      </c>
+      <c r="I324" s="1">
+        <v>40207</v>
+      </c>
+      <c r="K324" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L324" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="O324" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="325" spans="1:15">
+      <c r="A325">
+        <v>324</v>
+      </c>
+      <c r="B325" t="s">
+        <v>13</v>
+      </c>
+      <c r="C325">
+        <v>62</v>
+      </c>
+      <c r="D325" t="s">
+        <v>345</v>
+      </c>
+      <c r="E325" t="s">
+        <v>566</v>
+      </c>
+      <c r="H325" s="1">
+        <v>40209</v>
+      </c>
+      <c r="I325" s="1">
+        <v>40210</v>
+      </c>
+      <c r="K325" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L325" t="s">
+        <v>626</v>
+      </c>
+      <c r="O325" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="326" spans="1:15">
+      <c r="A326">
+        <v>325</v>
+      </c>
+      <c r="B326" t="s">
+        <v>13</v>
+      </c>
+      <c r="C326">
+        <v>59</v>
+      </c>
+      <c r="D326" t="s">
+        <v>421</v>
+      </c>
+      <c r="E326" t="s">
+        <v>345</v>
+      </c>
+      <c r="H326" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I326" s="1">
+        <v>40209</v>
+      </c>
+      <c r="K326" s="1">
+        <v>40216</v>
+      </c>
+      <c r="L326" t="s">
+        <v>627</v>
+      </c>
+      <c r="O326" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="327" spans="1:15">
+      <c r="A327">
+        <v>326</v>
+      </c>
+      <c r="B327" t="s">
+        <v>13</v>
+      </c>
+      <c r="C327">
+        <v>53</v>
+      </c>
+      <c r="D327" t="s">
+        <v>28</v>
+      </c>
+      <c r="E327" t="s">
+        <v>476</v>
+      </c>
+      <c r="H327" s="1">
+        <v>40209</v>
+      </c>
+      <c r="I327" s="1">
+        <v>40216</v>
+      </c>
+      <c r="K327" s="1">
+        <v>40217</v>
+      </c>
+      <c r="L327" t="s">
+        <v>628</v>
+      </c>
+      <c r="O327" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="328" spans="1:15">
+      <c r="A328">
+        <v>327</v>
+      </c>
+      <c r="B328" t="s">
+        <v>13</v>
+      </c>
+      <c r="C328">
+        <v>61</v>
+      </c>
+      <c r="D328" t="s">
+        <v>45</v>
+      </c>
+      <c r="E328" t="s">
+        <v>52</v>
+      </c>
+      <c r="H328" s="1">
+        <v>40206</v>
+      </c>
+      <c r="I328" s="1">
+        <v>40210</v>
+      </c>
+      <c r="K328" s="1">
+        <v>40217</v>
+      </c>
+      <c r="L328" t="s">
+        <v>629</v>
+      </c>
+      <c r="O328" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="329" spans="1:15">
+      <c r="A329">
+        <v>328</v>
+      </c>
+      <c r="B329" t="s">
+        <v>13</v>
+      </c>
+      <c r="C329">
+        <v>38</v>
+      </c>
+      <c r="D329" t="s">
+        <v>319</v>
+      </c>
+      <c r="E329" t="s">
+        <v>215</v>
+      </c>
+      <c r="H329" s="1">
+        <v>40204</v>
+      </c>
+      <c r="I329" s="1">
+        <v>40210</v>
+      </c>
+      <c r="K329" s="1">
+        <v>40217</v>
+      </c>
+      <c r="L329" t="s">
+        <v>630</v>
+      </c>
+      <c r="O329" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="330" spans="1:15">
+      <c r="A330">
+        <v>329</v>
+      </c>
+      <c r="B330" t="s">
+        <v>22</v>
+      </c>
+      <c r="C330">
+        <v>81</v>
+      </c>
+      <c r="D330" t="s">
+        <v>369</v>
+      </c>
+      <c r="E330" t="s">
+        <v>345</v>
+      </c>
+      <c r="H330" s="1">
+        <v>40208</v>
+      </c>
+      <c r="I330" s="1">
+        <v>40215</v>
+      </c>
+      <c r="J330" s="1">
+        <v>40215</v>
+      </c>
+      <c r="K330" s="1">
+        <v>40218</v>
+      </c>
+      <c r="L330" t="s">
+        <v>631</v>
+      </c>
+      <c r="N330" t="s">
+        <v>428</v>
+      </c>
+      <c r="O330" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="331" spans="1:15">
+      <c r="A331">
+        <v>330</v>
+      </c>
+      <c r="B331" t="s">
+        <v>13</v>
+      </c>
+      <c r="C331">
+        <v>11</v>
+      </c>
+      <c r="D331" t="s">
+        <v>566</v>
+      </c>
+      <c r="E331" t="s">
+        <v>345</v>
+      </c>
+      <c r="H331" s="1">
+        <v>40213</v>
+      </c>
+      <c r="I331" s="1">
+        <v>40213</v>
+      </c>
+      <c r="K331" s="1">
+        <v>40218</v>
+      </c>
+      <c r="L331" t="s">
+        <v>632</v>
+      </c>
+      <c r="O331" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="332" spans="1:15">
+      <c r="A332">
+        <v>331</v>
+      </c>
+      <c r="B332" t="s">
+        <v>13</v>
+      </c>
+      <c r="C332">
+        <v>68</v>
+      </c>
+      <c r="D332" t="s">
+        <v>45</v>
+      </c>
+      <c r="E332" t="s">
+        <v>394</v>
+      </c>
+      <c r="H332" s="1">
+        <v>40213</v>
+      </c>
+      <c r="I332" s="1">
+        <v>40215</v>
+      </c>
+      <c r="K332" s="1">
+        <v>40218</v>
+      </c>
+      <c r="L332" t="s">
+        <v>633</v>
+      </c>
+      <c r="O332" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="333" spans="1:15">
+      <c r="A333">
+        <v>332</v>
+      </c>
+      <c r="B333" t="s">
+        <v>13</v>
+      </c>
+      <c r="C333">
+        <v>66</v>
+      </c>
+      <c r="D333" t="s">
+        <v>634</v>
+      </c>
+      <c r="E333" t="s">
+        <v>23</v>
+      </c>
+      <c r="H333" s="1">
+        <v>40178</v>
+      </c>
+      <c r="I333" s="1">
+        <v>40184</v>
+      </c>
+      <c r="K333" s="1">
+        <v>40218</v>
+      </c>
+      <c r="L333" t="s">
+        <v>635</v>
+      </c>
+      <c r="O333" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="334" spans="1:15">
+      <c r="A334">
+        <v>333</v>
+      </c>
+      <c r="B334" t="s">
+        <v>13</v>
+      </c>
+      <c r="C334">
+        <v>67</v>
+      </c>
+      <c r="D334" t="s">
+        <v>45</v>
+      </c>
+      <c r="E334" t="s">
+        <v>239</v>
+      </c>
+      <c r="H334" s="1">
+        <v>40211</v>
+      </c>
+      <c r="I334" s="1">
+        <v>40216</v>
+      </c>
+      <c r="K334" s="1">
+        <v>40219</v>
+      </c>
+      <c r="L334" t="s">
+        <v>636</v>
+      </c>
+      <c r="O334" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="335" spans="1:15">
+      <c r="A335">
+        <v>334</v>
+      </c>
+      <c r="B335" t="s">
+        <v>22</v>
+      </c>
+      <c r="C335">
+        <v>47</v>
+      </c>
+      <c r="D335" t="s">
+        <v>45</v>
+      </c>
+      <c r="E335" t="s">
+        <v>164</v>
+      </c>
+      <c r="H335" s="1">
+        <v>40211</v>
+      </c>
+      <c r="I335" s="1">
+        <v>40215</v>
+      </c>
+      <c r="K335" s="1">
+        <v>40219</v>
+      </c>
+      <c r="L335" t="s">
+        <v>637</v>
+      </c>
+      <c r="O335" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="336" spans="1:15">
+      <c r="A336">
+        <v>335</v>
+      </c>
+      <c r="B336" t="s">
+        <v>13</v>
+      </c>
+      <c r="C336">
+        <v>62</v>
+      </c>
+      <c r="D336" t="s">
+        <v>45</v>
+      </c>
+      <c r="E336" t="s">
+        <v>310</v>
+      </c>
+      <c r="H336" s="1">
+        <v>40206</v>
+      </c>
+      <c r="I336" s="1">
+        <v>40214</v>
+      </c>
+      <c r="K336" s="1">
+        <v>40219</v>
+      </c>
+      <c r="L336" t="s">
+        <v>638</v>
+      </c>
+      <c r="O336" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="337" spans="1:15">
+      <c r="A337">
+        <v>336</v>
+      </c>
+      <c r="B337" t="s">
+        <v>13</v>
+      </c>
+      <c r="C337">
+        <v>56</v>
+      </c>
+      <c r="D337" t="s">
+        <v>23</v>
+      </c>
+      <c r="E337" t="s">
+        <v>639</v>
+      </c>
+      <c r="H337" s="1">
+        <v>40211</v>
+      </c>
+      <c r="I337" s="1">
+        <v>40215</v>
+      </c>
+      <c r="J337" s="1">
+        <v>40215</v>
+      </c>
+      <c r="K337" s="1">
+        <v>40219</v>
+      </c>
+      <c r="L337" t="s">
+        <v>640</v>
+      </c>
+      <c r="N337" t="s">
+        <v>428</v>
+      </c>
+      <c r="O337" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="338" spans="1:15">
+      <c r="A338">
+        <v>337</v>
+      </c>
+      <c r="B338" t="s">
+        <v>22</v>
+      </c>
+      <c r="C338">
+        <v>5</v>
+      </c>
+      <c r="D338" t="s">
+        <v>345</v>
+      </c>
+      <c r="E338" t="s">
+        <v>421</v>
+      </c>
+      <c r="H338" s="1">
+        <v>40209</v>
+      </c>
+      <c r="I338" s="1">
+        <v>40211</v>
+      </c>
+      <c r="K338" s="1">
+        <v>40219</v>
+      </c>
+      <c r="L338" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="O338" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="339" spans="1:15">
+      <c r="A339">
+        <v>338</v>
+      </c>
+      <c r="B339" t="s">
+        <v>13</v>
+      </c>
+      <c r="C339">
+        <v>70</v>
+      </c>
+      <c r="D339" t="s">
+        <v>45</v>
+      </c>
+      <c r="E339" t="s">
+        <v>52</v>
+      </c>
+      <c r="H339" s="1">
+        <v>40212</v>
+      </c>
+      <c r="I339" s="1">
+        <v>40213</v>
+      </c>
+      <c r="K339" s="1">
+        <v>40220</v>
+      </c>
+      <c r="L339" s="11" t="s">
+        <v>642</v>
+      </c>
+      <c r="O339" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="340" spans="1:15">
+      <c r="A340">
+        <v>339</v>
+      </c>
+      <c r="B340" t="s">
+        <v>13</v>
+      </c>
+      <c r="C340">
+        <v>23</v>
+      </c>
+      <c r="D340" t="s">
+        <v>215</v>
+      </c>
+      <c r="E340" t="s">
+        <v>585</v>
+      </c>
+      <c r="H340" s="1">
+        <v>40216</v>
+      </c>
+      <c r="I340" s="1">
+        <v>40217</v>
+      </c>
+      <c r="K340" s="1">
+        <v>40220</v>
+      </c>
+      <c r="L340" t="s">
+        <v>643</v>
+      </c>
+      <c r="O340" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="341" spans="1:15">
+      <c r="A341">
+        <v>340</v>
+      </c>
+      <c r="B341" t="s">
+        <v>13</v>
+      </c>
+      <c r="C341">
+        <v>65</v>
+      </c>
+      <c r="D341" t="s">
+        <v>370</v>
+      </c>
+      <c r="E341" t="s">
+        <v>370</v>
+      </c>
+      <c r="H341" s="1">
+        <v>40216</v>
+      </c>
+      <c r="I341" s="1">
+        <v>40219</v>
+      </c>
+      <c r="K341" s="1">
+        <v>40220</v>
+      </c>
+      <c r="L341" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="O341" t="s">
+        <v>646</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Some provinces/cities in the wrong order
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="682">
   <si>
     <t>gender</t>
   </si>
@@ -3412,10 +3412,10 @@
   <dimension ref="A1:S367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F316" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F313" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="L376" sqref="L376"/>
+      <selection pane="bottomRight" activeCell="F358" sqref="F358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14748,10 +14748,10 @@
         <v>48</v>
       </c>
       <c r="D324" t="s">
+        <v>345</v>
+      </c>
+      <c r="E324" t="s">
         <v>566</v>
-      </c>
-      <c r="E324" t="s">
-        <v>345</v>
       </c>
       <c r="H324" s="1">
         <v>40205</v>
@@ -14812,10 +14812,10 @@
         <v>59</v>
       </c>
       <c r="D326" t="s">
+        <v>345</v>
+      </c>
+      <c r="E326" t="s">
         <v>421</v>
-      </c>
-      <c r="E326" t="s">
-        <v>345</v>
       </c>
       <c r="H326" s="1">
         <v>40204</v>
@@ -14908,10 +14908,10 @@
         <v>38</v>
       </c>
       <c r="D329" t="s">
+        <v>215</v>
+      </c>
+      <c r="E329" t="s">
         <v>319</v>
-      </c>
-      <c r="E329" t="s">
-        <v>215</v>
       </c>
       <c r="H329" s="1">
         <v>40204</v>
@@ -14940,10 +14940,10 @@
         <v>81</v>
       </c>
       <c r="D330" t="s">
+        <v>345</v>
+      </c>
+      <c r="E330" t="s">
         <v>369</v>
-      </c>
-      <c r="E330" t="s">
-        <v>345</v>
       </c>
       <c r="H330" s="1">
         <v>40208</v>
@@ -14978,10 +14978,10 @@
         <v>11</v>
       </c>
       <c r="D331" t="s">
+        <v>345</v>
+      </c>
+      <c r="E331" t="s">
         <v>566</v>
-      </c>
-      <c r="E331" t="s">
-        <v>345</v>
       </c>
       <c r="H331" s="1">
         <v>40213</v>
@@ -15042,10 +15042,10 @@
         <v>66</v>
       </c>
       <c r="D333" t="s">
+        <v>23</v>
+      </c>
+      <c r="E333" t="s">
         <v>634</v>
-      </c>
-      <c r="E333" t="s">
-        <v>23</v>
       </c>
       <c r="H333" s="1">
         <v>40178</v>
@@ -15336,10 +15336,10 @@
         <v>84</v>
       </c>
       <c r="D342" t="s">
+        <v>45</v>
+      </c>
+      <c r="E342" t="s">
         <v>592</v>
-      </c>
-      <c r="E342" t="s">
-        <v>45</v>
       </c>
       <c r="H342" s="1">
         <v>40214</v>
@@ -15368,10 +15368,10 @@
         <v>58</v>
       </c>
       <c r="D343" t="s">
+        <v>45</v>
+      </c>
+      <c r="E343" t="s">
         <v>52</v>
-      </c>
-      <c r="E343" t="s">
-        <v>45</v>
       </c>
       <c r="H343" s="1">
         <v>40206</v>
@@ -15400,10 +15400,10 @@
         <v>46</v>
       </c>
       <c r="D344" t="s">
+        <v>45</v>
+      </c>
+      <c r="E344" t="s">
         <v>52</v>
-      </c>
-      <c r="E344" t="s">
-        <v>45</v>
       </c>
       <c r="H344" s="1">
         <v>40212</v>
@@ -15432,10 +15432,10 @@
         <v>8</v>
       </c>
       <c r="D345" t="s">
+        <v>345</v>
+      </c>
+      <c r="E345" t="s">
         <v>566</v>
-      </c>
-      <c r="E345" t="s">
-        <v>345</v>
       </c>
       <c r="H345" s="1">
         <v>40214</v>
@@ -15464,10 +15464,10 @@
         <v>46</v>
       </c>
       <c r="D346" t="s">
+        <v>345</v>
+      </c>
+      <c r="E346" t="s">
         <v>421</v>
-      </c>
-      <c r="E346" t="s">
-        <v>345</v>
       </c>
       <c r="H346" s="1">
         <v>40212</v>
@@ -15496,10 +15496,10 @@
         <v>65</v>
       </c>
       <c r="D347" t="s">
+        <v>345</v>
+      </c>
+      <c r="E347" t="s">
         <v>421</v>
-      </c>
-      <c r="E347" t="s">
-        <v>345</v>
       </c>
       <c r="H347" s="1">
         <v>40211</v>
@@ -15528,10 +15528,10 @@
         <v>19</v>
       </c>
       <c r="D348" t="s">
+        <v>215</v>
+      </c>
+      <c r="E348" t="s">
         <v>585</v>
-      </c>
-      <c r="E348" t="s">
-        <v>215</v>
       </c>
       <c r="H348" s="1">
         <v>40205</v>
@@ -15560,10 +15560,10 @@
         <v>67</v>
       </c>
       <c r="D349" t="s">
+        <v>345</v>
+      </c>
+      <c r="E349" t="s">
         <v>15</v>
-      </c>
-      <c r="E349" t="s">
-        <v>345</v>
       </c>
       <c r="G349" t="s">
         <v>655</v>
@@ -15595,10 +15595,10 @@
         <v>78</v>
       </c>
       <c r="D350" t="s">
+        <v>345</v>
+      </c>
+      <c r="E350" t="s">
         <v>421</v>
-      </c>
-      <c r="E350" t="s">
-        <v>345</v>
       </c>
       <c r="H350" s="1">
         <v>40215</v>
@@ -15633,10 +15633,10 @@
         <v>66</v>
       </c>
       <c r="D351" t="s">
+        <v>345</v>
+      </c>
+      <c r="E351" t="s">
         <v>526</v>
-      </c>
-      <c r="E351" t="s">
-        <v>345</v>
       </c>
       <c r="H351" s="1">
         <v>40204</v>
@@ -15665,10 +15665,10 @@
         <v>14</v>
       </c>
       <c r="D352" t="s">
+        <v>23</v>
+      </c>
+      <c r="E352" t="s">
         <v>634</v>
-      </c>
-      <c r="E352" t="s">
-        <v>23</v>
       </c>
       <c r="H352" s="1">
         <v>40220</v>
@@ -15697,10 +15697,10 @@
         <v>46</v>
       </c>
       <c r="D353" t="s">
+        <v>215</v>
+      </c>
+      <c r="E353" t="s">
         <v>585</v>
-      </c>
-      <c r="E353" t="s">
-        <v>215</v>
       </c>
       <c r="H353" s="1">
         <v>40208</v>
@@ -15729,10 +15729,10 @@
         <v>4</v>
       </c>
       <c r="D354" t="s">
+        <v>345</v>
+      </c>
+      <c r="E354" t="s">
         <v>421</v>
-      </c>
-      <c r="E354" t="s">
-        <v>345</v>
       </c>
       <c r="H354" s="1">
         <v>40219</v>
@@ -15761,10 +15761,10 @@
         <v>79</v>
       </c>
       <c r="D355" t="s">
+        <v>345</v>
+      </c>
+      <c r="E355" t="s">
         <v>421</v>
-      </c>
-      <c r="E355" t="s">
-        <v>345</v>
       </c>
       <c r="H355" s="1">
         <v>40212</v>
@@ -15793,10 +15793,10 @@
         <v>84</v>
       </c>
       <c r="D356" t="s">
+        <v>28</v>
+      </c>
+      <c r="E356" t="s">
         <v>665</v>
-      </c>
-      <c r="E356" t="s">
-        <v>28</v>
       </c>
       <c r="H356" s="1">
         <v>40212</v>
@@ -15825,10 +15825,10 @@
         <v>63</v>
       </c>
       <c r="D357" t="s">
+        <v>23</v>
+      </c>
+      <c r="E357" t="s">
         <v>667</v>
-      </c>
-      <c r="E357" t="s">
-        <v>23</v>
       </c>
       <c r="H357" s="1">
         <v>40217</v>
@@ -15857,10 +15857,10 @@
         <v>44</v>
       </c>
       <c r="D358" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="E358" s="9" t="s">
         <v>369</v>
-      </c>
-      <c r="E358" s="9" t="s">
-        <v>345</v>
       </c>
       <c r="G358" s="9"/>
       <c r="H358" s="10">
@@ -15896,10 +15896,10 @@
         <v>64</v>
       </c>
       <c r="D359" t="s">
+        <v>215</v>
+      </c>
+      <c r="E359" t="s">
         <v>319</v>
-      </c>
-      <c r="E359" t="s">
-        <v>215</v>
       </c>
       <c r="H359" s="1">
         <v>40217</v>
@@ -15928,10 +15928,10 @@
         <v>29</v>
       </c>
       <c r="D360" t="s">
+        <v>215</v>
+      </c>
+      <c r="E360" t="s">
         <v>344</v>
-      </c>
-      <c r="E360" t="s">
-        <v>215</v>
       </c>
       <c r="H360" s="1">
         <v>40216</v>
@@ -15960,10 +15960,10 @@
         <v>79</v>
       </c>
       <c r="D361" t="s">
+        <v>345</v>
+      </c>
+      <c r="E361" t="s">
         <v>398</v>
-      </c>
-      <c r="E361" t="s">
-        <v>345</v>
       </c>
       <c r="H361" s="1">
         <v>40218</v>
@@ -15992,10 +15992,10 @@
         <v>60</v>
       </c>
       <c r="D362" t="s">
+        <v>23</v>
+      </c>
+      <c r="E362" t="s">
         <v>673</v>
-      </c>
-      <c r="E362" t="s">
-        <v>23</v>
       </c>
       <c r="H362" s="1">
         <v>40221</v>
@@ -16024,10 +16024,10 @@
         <v>81</v>
       </c>
       <c r="D363" t="s">
+        <v>345</v>
+      </c>
+      <c r="E363" t="s">
         <v>421</v>
-      </c>
-      <c r="E363" t="s">
-        <v>345</v>
       </c>
       <c r="H363" s="1">
         <v>40215</v>
@@ -16056,10 +16056,10 @@
         <v>46</v>
       </c>
       <c r="D364" t="s">
+        <v>345</v>
+      </c>
+      <c r="E364" t="s">
         <v>566</v>
-      </c>
-      <c r="E364" t="s">
-        <v>345</v>
       </c>
       <c r="H364" s="1">
         <v>40221</v>
@@ -16088,10 +16088,10 @@
         <v>64</v>
       </c>
       <c r="D365" t="s">
+        <v>345</v>
+      </c>
+      <c r="E365" t="s">
         <v>421</v>
-      </c>
-      <c r="E365" t="s">
-        <v>345</v>
       </c>
       <c r="H365" s="1">
         <v>40223</v>
@@ -16120,10 +16120,10 @@
         <v>69</v>
       </c>
       <c r="D366" t="s">
+        <v>345</v>
+      </c>
+      <c r="E366" t="s">
         <v>526</v>
-      </c>
-      <c r="E366" t="s">
-        <v>345</v>
       </c>
       <c r="H366" s="1">
         <v>40218</v>
@@ -16151,9 +16151,11 @@
       <c r="C367" s="9">
         <v>50</v>
       </c>
-      <c r="D367" s="9"/>
+      <c r="D367" s="9" t="s">
+        <v>679</v>
+      </c>
       <c r="E367" s="9" t="s">
-        <v>679</v>
+        <v>15</v>
       </c>
       <c r="H367" s="10">
         <v>40223</v>

</xml_diff>

<commit_message>
Cleaning up some recent locations
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="681">
   <si>
     <t>gender</t>
   </si>
@@ -2014,9 +2014,6 @@
   </si>
   <si>
     <t>A 79 year-old farmer from Guangzhou City, Guangdong Province, who became ill on 4 February and was admitted to hospital the same day. He is currently in a critical condition.</t>
-  </si>
-  <si>
-    <t>Huai’an</t>
   </si>
   <si>
     <t>An 84 year-old man from Huai’an City, Jiangsu Province, who became ill on 4 February, and visited a community health center and then admitted to hospital on 9 February. He is currently in a severe condition. The patient has a history of exposure to poultry.</t>
@@ -2163,8 +2160,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="429">
+  <cellStyleXfs count="431">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2610,7 +2609,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="429">
+  <cellStyles count="431">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2825,6 +2824,7 @@
     <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3039,6 +3039,7 @@
     <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -3412,10 +3413,10 @@
   <dimension ref="A1:S367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F313" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F284" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="F358" sqref="F358"/>
+      <selection pane="bottomRight" activeCell="E356" sqref="E356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15796,7 +15797,7 @@
         <v>28</v>
       </c>
       <c r="E356" t="s">
-        <v>665</v>
+        <v>536</v>
       </c>
       <c r="H356" s="1">
         <v>40212</v>
@@ -15808,7 +15809,7 @@
         <v>40224</v>
       </c>
       <c r="L356" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="O356" s="1" t="s">
         <v>659</v>
@@ -15828,7 +15829,7 @@
         <v>23</v>
       </c>
       <c r="E357" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H357" s="1">
         <v>40217</v>
@@ -15840,7 +15841,7 @@
         <v>40224</v>
       </c>
       <c r="L357" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O357" s="1" t="s">
         <v>659</v>
@@ -15874,7 +15875,7 @@
         <v>40224</v>
       </c>
       <c r="L358" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="N358" s="9"/>
       <c r="O358" s="10" t="s">
@@ -15911,10 +15912,10 @@
         <v>40228</v>
       </c>
       <c r="L359" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O359" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="360" spans="1:19">
@@ -15943,10 +15944,10 @@
         <v>40228</v>
       </c>
       <c r="L360" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O360" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="361" spans="1:19">
@@ -15975,10 +15976,10 @@
         <v>40228</v>
       </c>
       <c r="L361" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="O361" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="362" spans="1:19">
@@ -15995,7 +15996,7 @@
         <v>23</v>
       </c>
       <c r="E362" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="H362" s="1">
         <v>40221</v>
@@ -16007,10 +16008,10 @@
         <v>40228</v>
       </c>
       <c r="L362" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O362" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="363" spans="1:19">
@@ -16039,10 +16040,10 @@
         <v>40228</v>
       </c>
       <c r="L363" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="O363" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="364" spans="1:19">
@@ -16071,10 +16072,10 @@
         <v>40229</v>
       </c>
       <c r="L364" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O364" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="365" spans="1:19">
@@ -16103,10 +16104,10 @@
         <v>40229</v>
       </c>
       <c r="L365" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O365" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="366" spans="1:19">
@@ -16135,10 +16136,10 @@
         <v>40229</v>
       </c>
       <c r="L366" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O366" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="367" spans="1:19">
@@ -16152,7 +16153,7 @@
         <v>50</v>
       </c>
       <c r="D367" s="9" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E367" s="9" t="s">
         <v>15</v>
@@ -16168,12 +16169,12 @@
         <v>40229</v>
       </c>
       <c r="L367" s="10" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M367" s="9"/>
       <c r="N367" s="9"/>
       <c r="O367" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="P367" s="9"/>
       <c r="Q367" s="9"/>

</xml_diff>

<commit_message>
9 new #H7N9 cases from @WHO with 4 new cities
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="47440" windowHeight="18700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cases.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="715">
   <si>
     <t>gender</t>
   </si>
@@ -2086,6 +2086,84 @@
   </si>
   <si>
     <t>The patient is a 71-year-old man from Foshan City in Guangdong Province. He became ill on 16 February, was hospitalised on 20 February and is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A two year-old girl from Jinhua City, Zhejiang Province. She became ill on 23 February, was hospitalised on 25 February and has a mild illness. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_03_03/en/</t>
+  </si>
+  <si>
+    <t>A 65 year-old woman from Guangzhou City, Guangdong Province. She became ill 17 February, was hospitalised on 24 February and is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 42 year-old man from Huaian City, Jiangsu Province. He became ill on 15 February, was hospitalised on 26 February and is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 77 year-old man from Yongzhou City, Hunan Province. He became ill on 20 February, was hospitalised on 25 February and is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A 41 year-old man from Yongzhou City, Hunan Province. He became ill on 17 February, was admitted to a hospital on 24 February and is currently in a critical condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A seven year-old girl from Jinhua City, Zhejiang Province. She became ill on 26 February, was hospitalised on 27 February and is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>A six year-old girl from Jinhua City, Zhejiang Province. She became ill on 26 February, was hospitalised on 27 February and is currently in a severe condition. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>Fuchuan</t>
+  </si>
+  <si>
+    <t>A 32 year-old man from Fuchuan County, Guangxi Province. He became ill on 20 February, was hospitalised on 26 February and is currently in a severe condition.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_03_05/en/</t>
+  </si>
+  <si>
+    <t>The patient is a 59 year-old man from Zhuhai City, Guangdong Province. He became ill on 26 February, was admitted to a hospital on 1 March and died on 2 March. The patient has a history of exposure to live poultry.</t>
+  </si>
+  <si>
+    <t>Zhuhai</t>
+  </si>
+  <si>
+    <t>The patient is an 18 month-old girl who developed mild fever. She consulted a doctor on 28 February, was admitted to a hospital on 1 March and was discharged from the hospital on 3 March in stable condition. Following laboratory-confirmation with avian influenza A(H7N9) virus infection on 4 March, the patient was admitted to another hospital. She is currently asymptomatic, with no fever. Initial epidemiological investigation revealed that the patient travelled to Foshan, Guangdong province from 5-27 February, where she visited a wet market with her mother. Further investigations into her travel and exposure history are ongoing, including tracing of all close contacts.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_03_07/en/</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_03_10/en/</t>
+  </si>
+  <si>
+    <t>A 59 year-old man originally from Taian city, Shandong Province currently lives in Wuxi City, Jiangsu Province. He became ill on 25 February, was admitted to a hospital on 3 March and is currently in a critical condition.</t>
+  </si>
+  <si>
+    <t>A 36 year-old man from Xuzhou City, Jiangsu Province. He became ill on 28 February, was admitted to a hospital on 2 March and is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 75 year-old man from Guangzhou City, Guangdong Province. He became ill on 19 February, was admitted to a hospital on 26 February and died on 1 March.</t>
+  </si>
+  <si>
+    <t>A 39 year- old man originally from Zhanjiang City, Guangdong Province, currently lives in Foshan City. He became ill on 27 February, was admitted to a hospital on 4 March 2014 and is currently is in a severe condition.</t>
+  </si>
+  <si>
+    <t>http://www.who.int/csr/don/2014_03_11b/en/</t>
+  </si>
+  <si>
+    <t>A 27 year-old man from Fuzhou City, Fujian Province. He became ill on 20 February, was admitted to a hospital on 27 February, and is currently in a stable condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 70 year-old man from Meizhou City, Guangdong Province. He became ill on 27 February, was admitted to a hospital on 3 March, and is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>A 76 year-old woman from Chaozhou City, Guangdong Province. She became ill on 1 March, was admitted to a hospital on 6 March, and is currently in a critical condition. The patient has a history of exposure to poultry.</t>
+  </si>
+  <si>
+    <t>Zhanjiang</t>
+  </si>
+  <si>
+    <t>Chaozhou</t>
   </si>
 </sst>
 </file>
@@ -2101,7 +2179,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2185,8 +2262,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="453">
+  <cellStyleXfs count="475">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2659,7 +2758,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="453">
+  <cellStyles count="475">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2886,6 +2985,17 @@
     <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3112,11 +3222,42 @@
     <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
@@ -3133,8 +3274,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S373" totalsRowShown="0">
-  <autoFilter ref="A1:S373"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S390" totalsRowShown="0">
+  <autoFilter ref="A1:S390"/>
   <sortState ref="A2:S367">
     <sortCondition ref="A1:A367"/>
   </sortState>
@@ -3485,13 +3626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S373"/>
+  <dimension ref="A1:S390"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F351" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="C373" sqref="C373"/>
+      <selection pane="bottomRight" activeCell="G388" sqref="G388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11091,7 +11232,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="218" spans="1:19" s="6" customFormat="1" ht="60">
+    <row r="218" spans="1:19" s="6" customFormat="1">
       <c r="A218">
         <v>217</v>
       </c>
@@ -11305,7 +11446,7 @@
       <c r="R223" s="6"/>
       <c r="S223" s="6"/>
     </row>
-    <row r="224" spans="1:19" ht="60">
+    <row r="224" spans="1:19">
       <c r="A224">
         <v>223</v>
       </c>
@@ -16517,6 +16658,620 @@
       <c r="Q373" s="6"/>
       <c r="R373" s="6"/>
       <c r="S373" s="6"/>
+    </row>
+    <row r="374" spans="1:19">
+      <c r="A374">
+        <v>373</v>
+      </c>
+      <c r="B374" t="s">
+        <v>22</v>
+      </c>
+      <c r="C374">
+        <v>2</v>
+      </c>
+      <c r="D374" t="s">
+        <v>45</v>
+      </c>
+      <c r="E374" t="s">
+        <v>592</v>
+      </c>
+      <c r="H374" s="1">
+        <v>40231</v>
+      </c>
+      <c r="I374" s="1">
+        <v>40233</v>
+      </c>
+      <c r="K374" s="1">
+        <v>40235</v>
+      </c>
+      <c r="L374" t="s">
+        <v>689</v>
+      </c>
+      <c r="O374" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="375" spans="1:19">
+      <c r="A375">
+        <v>374</v>
+      </c>
+      <c r="B375" t="s">
+        <v>22</v>
+      </c>
+      <c r="C375">
+        <v>65</v>
+      </c>
+      <c r="D375" t="s">
+        <v>345</v>
+      </c>
+      <c r="E375" t="s">
+        <v>421</v>
+      </c>
+      <c r="H375" s="1">
+        <v>40225</v>
+      </c>
+      <c r="I375" s="1">
+        <v>40232</v>
+      </c>
+      <c r="K375" s="1">
+        <v>40235</v>
+      </c>
+      <c r="L375" t="s">
+        <v>691</v>
+      </c>
+      <c r="O375" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="376" spans="1:19">
+      <c r="A376">
+        <v>375</v>
+      </c>
+      <c r="B376" t="s">
+        <v>13</v>
+      </c>
+      <c r="C376">
+        <v>42</v>
+      </c>
+      <c r="D376" t="s">
+        <v>28</v>
+      </c>
+      <c r="E376" t="s">
+        <v>536</v>
+      </c>
+      <c r="H376" s="1">
+        <v>40223</v>
+      </c>
+      <c r="I376" s="1">
+        <v>40234</v>
+      </c>
+      <c r="K376" s="1">
+        <v>40236</v>
+      </c>
+      <c r="L376" t="s">
+        <v>692</v>
+      </c>
+      <c r="O376" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="377" spans="1:19">
+      <c r="A377">
+        <v>376</v>
+      </c>
+      <c r="B377" t="s">
+        <v>13</v>
+      </c>
+      <c r="C377">
+        <v>77</v>
+      </c>
+      <c r="D377" t="s">
+        <v>215</v>
+      </c>
+      <c r="E377" t="s">
+        <v>572</v>
+      </c>
+      <c r="H377" s="1">
+        <v>40228</v>
+      </c>
+      <c r="I377" s="1">
+        <v>40233</v>
+      </c>
+      <c r="K377" s="1">
+        <v>40236</v>
+      </c>
+      <c r="L377" t="s">
+        <v>693</v>
+      </c>
+      <c r="O377" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="378" spans="1:19">
+      <c r="A378">
+        <v>377</v>
+      </c>
+      <c r="B378" t="s">
+        <v>13</v>
+      </c>
+      <c r="C378">
+        <v>41</v>
+      </c>
+      <c r="D378" t="s">
+        <v>215</v>
+      </c>
+      <c r="E378" t="s">
+        <v>572</v>
+      </c>
+      <c r="H378" s="1">
+        <v>40225</v>
+      </c>
+      <c r="I378" s="1">
+        <v>40232</v>
+      </c>
+      <c r="K378" s="1">
+        <v>40236</v>
+      </c>
+      <c r="L378" t="s">
+        <v>694</v>
+      </c>
+      <c r="O378" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="379" spans="1:19">
+      <c r="A379">
+        <v>378</v>
+      </c>
+      <c r="B379" t="s">
+        <v>22</v>
+      </c>
+      <c r="C379">
+        <v>7</v>
+      </c>
+      <c r="D379" t="s">
+        <v>45</v>
+      </c>
+      <c r="E379" t="s">
+        <v>592</v>
+      </c>
+      <c r="H379" s="1">
+        <v>40234</v>
+      </c>
+      <c r="I379" s="1">
+        <v>40235</v>
+      </c>
+      <c r="K379" s="1">
+        <v>40237</v>
+      </c>
+      <c r="L379" t="s">
+        <v>695</v>
+      </c>
+      <c r="O379" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="380" spans="1:19">
+      <c r="A380">
+        <v>379</v>
+      </c>
+      <c r="B380" t="s">
+        <v>22</v>
+      </c>
+      <c r="C380">
+        <v>6</v>
+      </c>
+      <c r="D380" t="s">
+        <v>45</v>
+      </c>
+      <c r="E380" t="s">
+        <v>592</v>
+      </c>
+      <c r="H380" s="1">
+        <v>40234</v>
+      </c>
+      <c r="I380" s="1">
+        <v>40235</v>
+      </c>
+      <c r="K380" s="1">
+        <v>40237</v>
+      </c>
+      <c r="L380" t="s">
+        <v>696</v>
+      </c>
+      <c r="O380" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="381" spans="1:19">
+      <c r="A381">
+        <v>380</v>
+      </c>
+      <c r="B381" t="s">
+        <v>13</v>
+      </c>
+      <c r="C381">
+        <v>32</v>
+      </c>
+      <c r="D381" t="s">
+        <v>559</v>
+      </c>
+      <c r="E381" t="s">
+        <v>697</v>
+      </c>
+      <c r="H381" s="1">
+        <v>40228</v>
+      </c>
+      <c r="I381" s="1">
+        <v>40234</v>
+      </c>
+      <c r="K381" s="1">
+        <v>40237</v>
+      </c>
+      <c r="L381" t="s">
+        <v>698</v>
+      </c>
+      <c r="O381" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="382" spans="1:19">
+      <c r="A382">
+        <v>381</v>
+      </c>
+      <c r="B382" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C382" s="6">
+        <v>59</v>
+      </c>
+      <c r="D382" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E382" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="F382" s="6"/>
+      <c r="G382" s="6"/>
+      <c r="H382" s="7">
+        <v>40234</v>
+      </c>
+      <c r="I382" s="7">
+        <v>40237</v>
+      </c>
+      <c r="J382" s="7">
+        <v>40238</v>
+      </c>
+      <c r="K382" s="7">
+        <v>40240</v>
+      </c>
+      <c r="L382" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="M382" s="6"/>
+      <c r="N382" s="6"/>
+      <c r="O382" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="P382" s="6"/>
+      <c r="Q382" s="6"/>
+      <c r="R382" s="6"/>
+      <c r="S382" s="6"/>
+    </row>
+    <row r="383" spans="1:19">
+      <c r="A383">
+        <v>382</v>
+      </c>
+      <c r="B383" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C383" s="6">
+        <v>1</v>
+      </c>
+      <c r="D383" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E383" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="F383" s="6"/>
+      <c r="G383" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="H383" s="7">
+        <v>40236</v>
+      </c>
+      <c r="I383" s="7">
+        <v>40237</v>
+      </c>
+      <c r="J383" s="7"/>
+      <c r="K383" s="7">
+        <v>40240</v>
+      </c>
+      <c r="L383" s="6" t="s">
+        <v>702</v>
+      </c>
+      <c r="M383" s="6"/>
+      <c r="N383" s="6"/>
+      <c r="O383" s="6" t="s">
+        <v>703</v>
+      </c>
+      <c r="P383" s="6"/>
+      <c r="Q383" s="6"/>
+      <c r="R383" s="6"/>
+      <c r="S383" s="6"/>
+    </row>
+    <row r="384" spans="1:19">
+      <c r="A384">
+        <v>383</v>
+      </c>
+      <c r="B384" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C384" s="6">
+        <v>59</v>
+      </c>
+      <c r="D384" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E384" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F384" s="6"/>
+      <c r="G384" s="6"/>
+      <c r="H384" s="7">
+        <v>40233</v>
+      </c>
+      <c r="I384" s="7">
+        <v>40238</v>
+      </c>
+      <c r="J384" s="7"/>
+      <c r="K384" s="7">
+        <v>40241</v>
+      </c>
+      <c r="L384" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="M384" s="6"/>
+      <c r="N384" s="6"/>
+      <c r="O384" s="6" t="s">
+        <v>704</v>
+      </c>
+      <c r="P384" s="6"/>
+      <c r="Q384" s="6"/>
+      <c r="R384" s="6"/>
+      <c r="S384" s="6"/>
+    </row>
+    <row r="385" spans="1:19">
+      <c r="A385">
+        <v>384</v>
+      </c>
+      <c r="B385" t="s">
+        <v>13</v>
+      </c>
+      <c r="C385">
+        <v>36</v>
+      </c>
+      <c r="D385" t="s">
+        <v>28</v>
+      </c>
+      <c r="E385" t="s">
+        <v>396</v>
+      </c>
+      <c r="H385" s="7">
+        <v>40236</v>
+      </c>
+      <c r="I385" s="7">
+        <v>40238</v>
+      </c>
+      <c r="K385" s="7">
+        <v>40241</v>
+      </c>
+      <c r="L385" t="s">
+        <v>706</v>
+      </c>
+      <c r="O385" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="386" spans="1:19">
+      <c r="A386">
+        <v>385</v>
+      </c>
+      <c r="B386" t="s">
+        <v>13</v>
+      </c>
+      <c r="C386">
+        <v>75</v>
+      </c>
+      <c r="D386" t="s">
+        <v>345</v>
+      </c>
+      <c r="E386" t="s">
+        <v>421</v>
+      </c>
+      <c r="H386" s="7">
+        <v>40227</v>
+      </c>
+      <c r="I386" s="1">
+        <v>40234</v>
+      </c>
+      <c r="J386" s="1">
+        <v>40237</v>
+      </c>
+      <c r="K386" s="7">
+        <v>40241</v>
+      </c>
+      <c r="L386" t="s">
+        <v>707</v>
+      </c>
+      <c r="O386" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="387" spans="1:19">
+      <c r="A387">
+        <v>386</v>
+      </c>
+      <c r="B387" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C387" s="6">
+        <v>39</v>
+      </c>
+      <c r="D387" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E387" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="F387" s="6"/>
+      <c r="G387" s="6"/>
+      <c r="H387" s="7">
+        <v>40235</v>
+      </c>
+      <c r="I387" s="7">
+        <v>40240</v>
+      </c>
+      <c r="J387" s="7"/>
+      <c r="K387" s="7">
+        <v>40242</v>
+      </c>
+      <c r="L387" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="M387" s="6"/>
+      <c r="N387" s="6"/>
+      <c r="O387" s="6" t="s">
+        <v>704</v>
+      </c>
+      <c r="P387" s="6"/>
+      <c r="Q387" s="6"/>
+      <c r="R387" s="6"/>
+      <c r="S387" s="6"/>
+    </row>
+    <row r="388" spans="1:19">
+      <c r="A388">
+        <v>387</v>
+      </c>
+      <c r="B388" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C388" s="6">
+        <v>27</v>
+      </c>
+      <c r="D388" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E388" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="F388" s="6"/>
+      <c r="G388" s="6"/>
+      <c r="H388" s="7">
+        <v>40228</v>
+      </c>
+      <c r="I388" s="7">
+        <v>40235</v>
+      </c>
+      <c r="J388" s="7"/>
+      <c r="K388" s="10">
+        <v>40241</v>
+      </c>
+      <c r="L388" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="M388" s="6"/>
+      <c r="N388" s="6"/>
+      <c r="O388" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="P388" s="6"/>
+      <c r="Q388" s="6"/>
+      <c r="R388" s="6"/>
+      <c r="S388" s="6"/>
+    </row>
+    <row r="389" spans="1:19">
+      <c r="A389">
+        <v>388</v>
+      </c>
+      <c r="B389" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C389" s="6">
+        <v>70</v>
+      </c>
+      <c r="D389" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E389" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="F389" s="6"/>
+      <c r="G389" s="6"/>
+      <c r="H389" s="7">
+        <v>40235</v>
+      </c>
+      <c r="I389" s="7">
+        <v>40239</v>
+      </c>
+      <c r="J389" s="7"/>
+      <c r="K389" s="10">
+        <v>40241</v>
+      </c>
+      <c r="L389" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="M389" s="6"/>
+      <c r="N389" s="6"/>
+      <c r="O389" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="P389" s="6"/>
+      <c r="Q389" s="6"/>
+      <c r="R389" s="6"/>
+      <c r="S389" s="6"/>
+    </row>
+    <row r="390" spans="1:19">
+      <c r="A390">
+        <v>389</v>
+      </c>
+      <c r="B390" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C390" s="6">
+        <v>76</v>
+      </c>
+      <c r="D390" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E390" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="F390" s="6"/>
+      <c r="G390" s="6"/>
+      <c r="H390" s="7">
+        <v>40237</v>
+      </c>
+      <c r="I390" s="7">
+        <v>40242</v>
+      </c>
+      <c r="J390" s="7"/>
+      <c r="K390" s="10">
+        <v>40241</v>
+      </c>
+      <c r="L390" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="M390" s="6"/>
+      <c r="N390" s="6"/>
+      <c r="O390" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="P390" s="6"/>
+      <c r="Q390" s="6"/>
+      <c r="R390" s="6"/>
+      <c r="S390" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>